<commit_message>
Enhance inventory file detection with improved title and data pattern recognition
</commit_message>
<xml_diff>
--- a/config/Program Requirements - PDM - NPI  for Audit.xlsx
+++ b/config/Program Requirements - PDM - NPI  for Audit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\picadocj\Desktop\audit_control-main\audit_control-main\audit_control-main\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229E60E6-7008-4C36-A554-BDD3011E02E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE6F8B1-C978-44B1-8D98-CCA1B8B4BD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8760" uniqueCount="2637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8788" uniqueCount="2638">
   <si>
     <t>Program Onboarding Date</t>
   </si>
@@ -8069,6 +8069,9 @@
   </si>
   <si>
     <t>40,132</t>
+  </si>
+  <si>
+    <t>22,122</t>
   </si>
 </sst>
 </file>
@@ -8136,22 +8139,25 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
-      <name val="VERDANA"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="ARIAL"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -8230,7 +8236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -8396,17 +8402,8 @@
     </xf>
     <xf numFmtId="3" fontId="11" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8746,8 +8743,8 @@
   </sheetPr>
   <dimension ref="A1:AJ461"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="A446" workbookViewId="0">
+      <selection activeCell="R458" sqref="R458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8933,7 +8930,7 @@
       <c r="Q2" s="66">
         <v>40</v>
       </c>
-      <c r="R2" s="67" t="s">
+      <c r="R2" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S2" s="3" t="s">
@@ -9013,7 +9010,7 @@
       <c r="Q3" s="66">
         <v>43</v>
       </c>
-      <c r="R3" s="68" t="s">
+      <c r="R3" s="13" t="s">
         <v>60</v>
       </c>
       <c r="S3" s="3" t="s">
@@ -9097,7 +9094,7 @@
       <c r="Q4" s="66">
         <v>73</v>
       </c>
-      <c r="R4" s="67" t="s">
+      <c r="R4" s="3" t="s">
         <v>70</v>
       </c>
       <c r="S4" s="3" t="s">
@@ -9189,7 +9186,7 @@
       <c r="Q5" s="66">
         <v>43</v>
       </c>
-      <c r="R5" s="67" t="s">
+      <c r="R5" s="3" t="s">
         <v>80</v>
       </c>
       <c r="S5" s="3" t="s">
@@ -9279,7 +9276,7 @@
       <c r="Q6" s="66">
         <v>43</v>
       </c>
-      <c r="R6" s="67" t="s">
+      <c r="R6" s="3" t="s">
         <v>80</v>
       </c>
       <c r="S6" s="3" t="s">
@@ -9363,7 +9360,7 @@
       <c r="Q7" s="66">
         <v>132</v>
       </c>
-      <c r="R7" s="67" t="s">
+      <c r="R7" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S7" s="3" t="s">
@@ -9437,7 +9434,7 @@
       <c r="Q8" s="66">
         <v>132</v>
       </c>
-      <c r="R8" s="67" t="s">
+      <c r="R8" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S8" s="3" t="s">
@@ -9499,7 +9496,7 @@
       <c r="Q9" s="66">
         <v>132</v>
       </c>
-      <c r="R9" s="67" t="s">
+      <c r="R9" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S9" s="3" t="s">
@@ -9567,7 +9564,7 @@
       <c r="Q10" s="66">
         <v>132</v>
       </c>
-      <c r="R10" s="67" t="s">
+      <c r="R10" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S10" s="3" t="s">
@@ -9647,7 +9644,7 @@
       <c r="Q11" s="66">
         <v>132</v>
       </c>
-      <c r="R11" s="67" t="s">
+      <c r="R11" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S11" s="3" t="s">
@@ -9713,7 +9710,7 @@
       <c r="Q12" s="66">
         <v>40</v>
       </c>
-      <c r="R12" s="67" t="s">
+      <c r="R12" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S12" s="3" t="s">
@@ -9803,7 +9800,7 @@
       <c r="Q13" s="66">
         <v>40</v>
       </c>
-      <c r="R13" s="67" t="s">
+      <c r="R13" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S13" s="3" t="s">
@@ -9869,7 +9866,7 @@
       <c r="Q14" s="66">
         <v>40</v>
       </c>
-      <c r="R14" s="67" t="s">
+      <c r="R14" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S14" s="3" t="s">
@@ -9931,7 +9928,7 @@
       <c r="Q15" s="66">
         <v>40</v>
       </c>
-      <c r="R15" s="67" t="s">
+      <c r="R15" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S15" s="3" t="s">
@@ -10015,7 +10012,7 @@
       <c r="Q16" s="66">
         <v>40</v>
       </c>
-      <c r="R16" s="67" t="s">
+      <c r="R16" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S16" s="3" t="s">
@@ -10103,7 +10100,7 @@
       <c r="Q17" s="66">
         <v>40</v>
       </c>
-      <c r="R17" s="67" t="s">
+      <c r="R17" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S17" s="3" t="s">
@@ -10195,7 +10192,7 @@
       <c r="Q18" s="66">
         <v>40</v>
       </c>
-      <c r="R18" s="67" t="s">
+      <c r="R18" s="3" t="s">
         <v>172</v>
       </c>
       <c r="S18" s="3" t="s">
@@ -10285,7 +10282,7 @@
       <c r="Q19" s="66">
         <v>40</v>
       </c>
-      <c r="R19" s="67" t="s">
+      <c r="R19" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S19" s="3" t="s">
@@ -10375,7 +10372,7 @@
       <c r="Q20" s="66">
         <v>43</v>
       </c>
-      <c r="R20" s="67" t="s">
+      <c r="R20" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S20" s="3" t="s">
@@ -10457,7 +10454,7 @@
       <c r="Q21" s="66">
         <v>40</v>
       </c>
-      <c r="R21" s="67" t="s">
+      <c r="R21" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S21" s="3" t="s">
@@ -10547,7 +10544,7 @@
       <c r="Q22" s="66">
         <v>132</v>
       </c>
-      <c r="R22" s="67" t="s">
+      <c r="R22" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S22" s="3" t="s">
@@ -10625,7 +10622,7 @@
       <c r="Q23" s="66">
         <v>43</v>
       </c>
-      <c r="R23" s="67" t="s">
+      <c r="R23" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S23" s="14" t="s">
@@ -10693,7 +10690,7 @@
       <c r="Q24" s="66">
         <v>40</v>
       </c>
-      <c r="R24" s="67" t="s">
+      <c r="R24" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S24" s="3" t="s">
@@ -10771,7 +10768,7 @@
       <c r="Q25" s="66">
         <v>132</v>
       </c>
-      <c r="R25" s="67" t="s">
+      <c r="R25" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S25" s="3" t="s">
@@ -10855,7 +10852,7 @@
       <c r="Q26" s="66">
         <v>132</v>
       </c>
-      <c r="R26" s="67" t="s">
+      <c r="R26" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S26" s="3" t="s">
@@ -10947,7 +10944,7 @@
       <c r="Q27" s="66">
         <v>132</v>
       </c>
-      <c r="R27" s="67" t="s">
+      <c r="R27" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S27" s="3" t="s">
@@ -11037,7 +11034,7 @@
       <c r="Q28" s="66">
         <v>132</v>
       </c>
-      <c r="R28" s="67" t="s">
+      <c r="R28" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S28" s="3" t="s">
@@ -11123,7 +11120,7 @@
       <c r="Q29" s="66">
         <v>40</v>
       </c>
-      <c r="R29" s="67" t="s">
+      <c r="R29" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S29" s="3" t="s">
@@ -11197,7 +11194,7 @@
       <c r="Q30" s="66">
         <v>40</v>
       </c>
-      <c r="R30" s="67" t="s">
+      <c r="R30" s="3" t="s">
         <v>267</v>
       </c>
       <c r="S30" s="3" t="s">
@@ -11273,7 +11270,7 @@
       <c r="Q31" s="66">
         <v>40</v>
       </c>
-      <c r="R31" s="67" t="s">
+      <c r="R31" s="3" t="s">
         <v>274</v>
       </c>
       <c r="S31" s="14" t="s">
@@ -11361,7 +11358,7 @@
       <c r="Q32" s="66">
         <v>132</v>
       </c>
-      <c r="R32" s="67" t="s">
+      <c r="R32" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S32" s="14" t="s">
@@ -11435,7 +11432,7 @@
       <c r="Q33" s="66">
         <v>40</v>
       </c>
-      <c r="R33" s="67" t="s">
+      <c r="R33" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S33" s="14" t="s">
@@ -11511,7 +11508,7 @@
       <c r="Q34" s="66">
         <v>40</v>
       </c>
-      <c r="R34" s="67" t="s">
+      <c r="R34" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S34" s="3" t="s">
@@ -11591,7 +11588,7 @@
       <c r="Q35" s="66">
         <v>40</v>
       </c>
-      <c r="R35" s="67" t="s">
+      <c r="R35" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S35" s="3" t="s">
@@ -11681,10 +11678,10 @@
       <c r="Q36" s="66">
         <v>73</v>
       </c>
-      <c r="R36" s="69" t="s">
+      <c r="R36" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="S36" s="3">
+      <c r="S36" s="14">
         <v>24</v>
       </c>
       <c r="T36" s="13" t="s">
@@ -11771,10 +11768,10 @@
       <c r="Q37" s="66">
         <v>73</v>
       </c>
-      <c r="R37" s="69" t="s">
+      <c r="R37" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="S37" s="3">
+      <c r="S37" s="14">
         <v>24</v>
       </c>
       <c r="T37" s="13" t="s">
@@ -11861,10 +11858,10 @@
       <c r="Q38" s="66">
         <v>73</v>
       </c>
-      <c r="R38" s="69" t="s">
+      <c r="R38" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="S38" s="3">
+      <c r="S38" s="14">
         <v>24</v>
       </c>
       <c r="T38" s="13" t="s">
@@ -11957,10 +11954,10 @@
       <c r="Q39" s="66">
         <v>73</v>
       </c>
-      <c r="R39" s="69" t="s">
+      <c r="R39" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="S39" s="3">
+      <c r="S39" s="14">
         <v>24</v>
       </c>
       <c r="T39" s="13" t="s">
@@ -12047,10 +12044,10 @@
       <c r="Q40" s="66">
         <v>73</v>
       </c>
-      <c r="R40" s="69" t="s">
+      <c r="R40" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="S40" s="3">
+      <c r="S40" s="14">
         <v>24</v>
       </c>
       <c r="T40" s="13" t="s">
@@ -12123,10 +12120,10 @@
       <c r="Q41" s="66">
         <v>122</v>
       </c>
-      <c r="R41" s="69" t="s">
+      <c r="R41" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="S41" s="3">
+      <c r="S41" s="14">
         <v>106</v>
       </c>
       <c r="T41" s="13" t="s">
@@ -12209,10 +12206,10 @@
       <c r="Q42" s="66">
         <v>73</v>
       </c>
-      <c r="R42" s="69" t="s">
+      <c r="R42" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="S42" s="3">
+      <c r="S42" s="14">
         <v>24</v>
       </c>
       <c r="T42" s="13" t="s">
@@ -12295,10 +12292,10 @@
       <c r="Q43" s="66">
         <v>73</v>
       </c>
-      <c r="R43" s="69" t="s">
+      <c r="R43" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="S43" s="3">
+      <c r="S43" s="14">
         <v>24</v>
       </c>
       <c r="T43" s="13" t="s">
@@ -12385,7 +12382,7 @@
       <c r="Q44" s="66">
         <v>40</v>
       </c>
-      <c r="R44" s="67" t="s">
+      <c r="R44" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S44" s="3" t="s">
@@ -12459,11 +12456,11 @@
       <c r="Q45" s="66">
         <v>131</v>
       </c>
-      <c r="R45" s="67" t="s">
+      <c r="R45" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S45" s="12">
-        <v>24100</v>
+      <c r="S45" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T45" s="13" t="s">
         <v>374</v>
@@ -12529,7 +12526,7 @@
       <c r="Q46" s="66">
         <v>73</v>
       </c>
-      <c r="R46" s="67" t="s">
+      <c r="R46" s="3" t="s">
         <v>380</v>
       </c>
       <c r="S46" s="14" t="s">
@@ -12615,7 +12612,7 @@
       <c r="Q47" s="66">
         <v>73</v>
       </c>
-      <c r="R47" s="67" t="s">
+      <c r="R47" s="3" t="s">
         <v>380</v>
       </c>
       <c r="S47" s="14" t="s">
@@ -12701,7 +12698,7 @@
       <c r="Q48" s="66">
         <v>73</v>
       </c>
-      <c r="R48" s="67" t="s">
+      <c r="R48" s="3" t="s">
         <v>380</v>
       </c>
       <c r="S48" s="14" t="s">
@@ -12791,7 +12788,7 @@
       <c r="Q49" s="66">
         <v>73</v>
       </c>
-      <c r="R49" s="67" t="s">
+      <c r="R49" s="3" t="s">
         <v>380</v>
       </c>
       <c r="S49" s="14" t="s">
@@ -12879,7 +12876,7 @@
       <c r="Q50" s="66">
         <v>73</v>
       </c>
-      <c r="R50" s="67" t="s">
+      <c r="R50" s="3" t="s">
         <v>380</v>
       </c>
       <c r="S50" s="14" t="s">
@@ -12949,7 +12946,7 @@
       <c r="Q51" s="66">
         <v>73</v>
       </c>
-      <c r="R51" s="67" t="s">
+      <c r="R51" s="3" t="s">
         <v>407</v>
       </c>
       <c r="S51" s="14" t="s">
@@ -13019,7 +13016,7 @@
       <c r="Q52" s="66">
         <v>73</v>
       </c>
-      <c r="R52" s="67" t="s">
+      <c r="R52" s="3" t="s">
         <v>313</v>
       </c>
       <c r="S52" s="14" t="s">
@@ -13099,7 +13096,7 @@
       <c r="Q53" s="66">
         <v>73</v>
       </c>
-      <c r="R53" s="67" t="s">
+      <c r="R53" s="3" t="s">
         <v>313</v>
       </c>
       <c r="S53" s="14" t="s">
@@ -13181,7 +13178,7 @@
       <c r="Q54" s="66">
         <v>40</v>
       </c>
-      <c r="R54" s="67" t="s">
+      <c r="R54" s="3" t="s">
         <v>421</v>
       </c>
       <c r="S54" s="3" t="s">
@@ -13255,7 +13252,7 @@
       <c r="Q55" s="66">
         <v>40</v>
       </c>
-      <c r="R55" s="67" t="s">
+      <c r="R55" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S55" s="3" t="s">
@@ -13337,7 +13334,7 @@
       <c r="Q56" s="66">
         <v>40</v>
       </c>
-      <c r="R56" s="67" t="s">
+      <c r="R56" s="3" t="s">
         <v>421</v>
       </c>
       <c r="S56" s="3" t="s">
@@ -13409,7 +13406,7 @@
       <c r="Q57" s="66">
         <v>40</v>
       </c>
-      <c r="R57" s="67" t="s">
+      <c r="R57" s="3" t="s">
         <v>421</v>
       </c>
       <c r="S57" s="3" t="s">
@@ -13495,7 +13492,7 @@
       <c r="Q58" s="66">
         <v>40</v>
       </c>
-      <c r="R58" s="67" t="s">
+      <c r="R58" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S58" s="3" t="s">
@@ -13567,7 +13564,7 @@
       <c r="Q59" s="66">
         <v>132</v>
       </c>
-      <c r="R59" s="70" t="s">
+      <c r="R59" s="67" t="s">
         <v>464</v>
       </c>
       <c r="S59" s="63" t="s">
@@ -13657,7 +13654,7 @@
       <c r="Q60" s="66">
         <v>40</v>
       </c>
-      <c r="R60" s="67" t="s">
+      <c r="R60" s="3" t="s">
         <v>477</v>
       </c>
       <c r="S60" s="3" t="s">
@@ -13729,7 +13726,7 @@
       <c r="Q61" s="66">
         <v>40</v>
       </c>
-      <c r="R61" s="67" t="s">
+      <c r="R61" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S61" s="3" t="s">
@@ -13811,7 +13808,7 @@
       <c r="Q62" s="66">
         <v>40</v>
       </c>
-      <c r="R62" s="67" t="s">
+      <c r="R62" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S62" s="3" t="s">
@@ -13901,7 +13898,7 @@
       <c r="Q63" s="66">
         <v>40</v>
       </c>
-      <c r="R63" s="67" t="s">
+      <c r="R63" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S63" s="3" t="s">
@@ -13991,7 +13988,7 @@
       <c r="Q64" s="66">
         <v>40</v>
       </c>
-      <c r="R64" s="67" t="s">
+      <c r="R64" s="3" t="s">
         <v>508</v>
       </c>
       <c r="S64" s="3" t="s">
@@ -14077,7 +14074,7 @@
       <c r="Q65" s="66">
         <v>40</v>
       </c>
-      <c r="R65" s="67" t="s">
+      <c r="R65" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S65" s="3" t="s">
@@ -14159,7 +14156,7 @@
       <c r="Q66" s="66">
         <v>40</v>
       </c>
-      <c r="R66" s="67" t="s">
+      <c r="R66" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S66" s="3" t="s">
@@ -14249,7 +14246,7 @@
       <c r="Q67" s="66">
         <v>40</v>
       </c>
-      <c r="R67" s="67" t="s">
+      <c r="R67" s="3" t="s">
         <v>421</v>
       </c>
       <c r="S67" s="3" t="s">
@@ -14311,7 +14308,7 @@
       <c r="Q68" s="66">
         <v>40</v>
       </c>
-      <c r="R68" s="67" t="s">
+      <c r="R68" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S68" s="3" t="s">
@@ -14393,7 +14390,7 @@
       <c r="Q69" s="66">
         <v>40</v>
       </c>
-      <c r="R69" s="67" t="s">
+      <c r="R69" s="3" t="s">
         <v>421</v>
       </c>
       <c r="S69" s="3" t="s">
@@ -14483,7 +14480,7 @@
       <c r="Q70" s="66">
         <v>40</v>
       </c>
-      <c r="R70" s="67" t="s">
+      <c r="R70" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S70" s="3" t="s">
@@ -14579,7 +14576,7 @@
       <c r="Q71" s="66">
         <v>40</v>
       </c>
-      <c r="R71" s="67" t="s">
+      <c r="R71" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S71" s="3" t="s">
@@ -14655,7 +14652,7 @@
       <c r="Q72" s="66">
         <v>40</v>
       </c>
-      <c r="R72" s="67" t="s">
+      <c r="R72" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S72" s="3" t="s">
@@ -14741,7 +14738,7 @@
       <c r="Q73" s="66">
         <v>40</v>
       </c>
-      <c r="R73" s="67" t="s">
+      <c r="R73" s="3" t="s">
         <v>579</v>
       </c>
       <c r="S73" s="14" t="s">
@@ -14827,7 +14824,7 @@
       <c r="Q74" s="66">
         <v>40</v>
       </c>
-      <c r="R74" s="67" t="s">
+      <c r="R74" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S74" s="3" t="s">
@@ -14913,7 +14910,7 @@
       <c r="Q75" s="66">
         <v>87</v>
       </c>
-      <c r="R75" s="67" t="s">
+      <c r="R75" s="3" t="s">
         <v>588</v>
       </c>
       <c r="S75" s="14" t="s">
@@ -15001,7 +14998,7 @@
       <c r="Q76" s="66">
         <v>40</v>
       </c>
-      <c r="R76" s="67" t="s">
+      <c r="R76" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S76" s="3" t="s">
@@ -15085,7 +15082,7 @@
       <c r="Q77" s="66">
         <v>40</v>
       </c>
-      <c r="R77" s="67" t="s">
+      <c r="R77" s="3" t="s">
         <v>588</v>
       </c>
       <c r="S77" s="14" t="s">
@@ -15171,7 +15168,7 @@
       <c r="Q78" s="66">
         <v>40</v>
       </c>
-      <c r="R78" s="67" t="s">
+      <c r="R78" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S78" s="3" t="s">
@@ -15259,7 +15256,7 @@
       <c r="Q79" s="66">
         <v>40</v>
       </c>
-      <c r="R79" s="67" t="s">
+      <c r="R79" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S79" s="3" t="s">
@@ -15337,7 +15334,7 @@
       <c r="Q80" s="66">
         <v>40</v>
       </c>
-      <c r="R80" s="67" t="s">
+      <c r="R80" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S80" s="3" t="s">
@@ -15419,7 +15416,7 @@
       <c r="Q81" s="66">
         <v>40</v>
       </c>
-      <c r="R81" s="67" t="s">
+      <c r="R81" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S81" s="3" t="s">
@@ -15485,7 +15482,7 @@
       <c r="Q82" s="66">
         <v>40</v>
       </c>
-      <c r="R82" s="67" t="s">
+      <c r="R82" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S82" s="3" t="s">
@@ -15539,7 +15536,7 @@
       <c r="Q83" s="66">
         <v>40</v>
       </c>
-      <c r="R83" s="67" t="s">
+      <c r="R83" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S83" s="3" t="s">
@@ -15607,7 +15604,7 @@
       <c r="Q84" s="66">
         <v>40</v>
       </c>
-      <c r="R84" s="67" t="s">
+      <c r="R84" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S84" s="3" t="s">
@@ -15691,7 +15688,7 @@
       <c r="Q85" s="66">
         <v>40</v>
       </c>
-      <c r="R85" s="67" t="s">
+      <c r="R85" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S85" s="3" t="s">
@@ -15775,7 +15772,7 @@
       <c r="Q86" s="66">
         <v>40</v>
       </c>
-      <c r="R86" s="67" t="s">
+      <c r="R86" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S86" s="3" t="s">
@@ -15861,7 +15858,7 @@
       <c r="Q87" s="66">
         <v>132</v>
       </c>
-      <c r="R87" s="67" t="s">
+      <c r="R87" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S87" s="3" t="s">
@@ -15937,7 +15934,7 @@
       <c r="Q88" s="66">
         <v>40</v>
       </c>
-      <c r="R88" s="67" t="s">
+      <c r="R88" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S88" s="3" t="s">
@@ -16021,7 +16018,7 @@
       <c r="Q89" s="66">
         <v>40</v>
       </c>
-      <c r="R89" s="67" t="s">
+      <c r="R89" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S89" s="3" t="s">
@@ -16107,8 +16104,8 @@
       <c r="Q90" s="66">
         <v>122</v>
       </c>
-      <c r="R90" s="67">
-        <v>22122</v>
+      <c r="R90" s="14" t="s">
+        <v>2637</v>
       </c>
       <c r="S90" s="14" t="s">
         <v>683</v>
@@ -16169,7 +16166,7 @@
       <c r="Q91" s="66">
         <v>40</v>
       </c>
-      <c r="R91" s="67" t="s">
+      <c r="R91" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S91" s="3" t="s">
@@ -16247,7 +16244,7 @@
       <c r="Q92" s="66">
         <v>132</v>
       </c>
-      <c r="R92" s="67" t="s">
+      <c r="R92" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S92" s="3" t="s">
@@ -16323,7 +16320,7 @@
       <c r="Q93" s="66">
         <v>85</v>
       </c>
-      <c r="R93" s="67" t="s">
+      <c r="R93" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S93" s="14" t="s">
@@ -16389,7 +16386,7 @@
       <c r="Q94" s="66">
         <v>131</v>
       </c>
-      <c r="R94" s="67" t="s">
+      <c r="R94" s="3" t="s">
         <v>313</v>
       </c>
       <c r="S94" s="14" t="s">
@@ -16473,7 +16470,7 @@
       <c r="Q95" s="66">
         <v>40</v>
       </c>
-      <c r="R95" s="67" t="s">
+      <c r="R95" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S95" s="3" t="s">
@@ -16561,7 +16558,7 @@
       <c r="Q96" s="66">
         <v>40</v>
       </c>
-      <c r="R96" s="67" t="s">
+      <c r="R96" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S96" s="3" t="s">
@@ -16631,7 +16628,7 @@
       <c r="Q97" s="66">
         <v>40</v>
       </c>
-      <c r="R97" s="67" t="s">
+      <c r="R97" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S97" s="3" t="s">
@@ -16711,7 +16708,7 @@
       <c r="Q98" s="66">
         <v>40</v>
       </c>
-      <c r="R98" s="67" t="s">
+      <c r="R98" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S98" s="3" t="s">
@@ -16795,7 +16792,7 @@
       <c r="Q99" s="66">
         <v>40</v>
       </c>
-      <c r="R99" s="67" t="s">
+      <c r="R99" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S99" s="3" t="s">
@@ -16879,7 +16876,7 @@
       <c r="Q100" s="66">
         <v>40</v>
       </c>
-      <c r="R100" s="67" t="s">
+      <c r="R100" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S100" s="3" t="s">
@@ -16955,7 +16952,7 @@
       <c r="Q101" s="66">
         <v>40</v>
       </c>
-      <c r="R101" s="67" t="s">
+      <c r="R101" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S101" s="3" t="s">
@@ -17037,7 +17034,7 @@
       <c r="Q102" s="66">
         <v>132</v>
       </c>
-      <c r="R102" s="67" t="s">
+      <c r="R102" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S102" s="3" t="s">
@@ -17129,7 +17126,7 @@
       <c r="Q103" s="66">
         <v>40</v>
       </c>
-      <c r="R103" s="67" t="s">
+      <c r="R103" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S103" s="3" t="s">
@@ -17217,7 +17214,7 @@
       <c r="Q104" s="66">
         <v>40</v>
       </c>
-      <c r="R104" s="67" t="s">
+      <c r="R104" s="3" t="s">
         <v>267</v>
       </c>
       <c r="S104" s="3" t="s">
@@ -17299,7 +17296,7 @@
       <c r="Q105" s="66">
         <v>40</v>
       </c>
-      <c r="R105" s="67" t="s">
+      <c r="R105" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S105" s="3" t="s">
@@ -17383,7 +17380,7 @@
       <c r="Q106" s="66">
         <v>40</v>
       </c>
-      <c r="R106" s="67" t="s">
+      <c r="R106" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S106" s="3" t="s">
@@ -17467,7 +17464,7 @@
       <c r="Q107" s="66">
         <v>40</v>
       </c>
-      <c r="R107" s="67" t="s">
+      <c r="R107" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S107" s="3" t="s">
@@ -17539,7 +17536,7 @@
       <c r="Q108" s="66">
         <v>40</v>
       </c>
-      <c r="R108" s="67" t="s">
+      <c r="R108" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S108" s="3" t="s">
@@ -17633,7 +17630,7 @@
       <c r="Q109" s="66">
         <v>40</v>
       </c>
-      <c r="R109" s="67" t="s">
+      <c r="R109" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S109" s="3" t="s">
@@ -17715,7 +17712,7 @@
       <c r="Q110" s="66">
         <v>40</v>
       </c>
-      <c r="R110" s="67" t="s">
+      <c r="R110" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S110" s="3" t="s">
@@ -17795,7 +17792,7 @@
       <c r="Q111" s="66">
         <v>122</v>
       </c>
-      <c r="R111" s="67" t="s">
+      <c r="R111" s="3" t="s">
         <v>815</v>
       </c>
       <c r="S111" s="12">
@@ -17867,7 +17864,7 @@
       <c r="Q112" s="66">
         <v>40</v>
       </c>
-      <c r="R112" s="67" t="s">
+      <c r="R112" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S112" s="3" t="s">
@@ -17953,7 +17950,7 @@
       <c r="Q113" s="66">
         <v>40</v>
       </c>
-      <c r="R113" s="67" t="s">
+      <c r="R113" s="3" t="s">
         <v>267</v>
       </c>
       <c r="S113" s="3" t="s">
@@ -18039,7 +18036,7 @@
       <c r="Q114" s="66">
         <v>73</v>
       </c>
-      <c r="R114" s="67" t="s">
+      <c r="R114" s="3" t="s">
         <v>313</v>
       </c>
       <c r="S114" s="12">
@@ -18127,7 +18124,7 @@
       <c r="Q115" s="66">
         <v>40</v>
       </c>
-      <c r="R115" s="67" t="s">
+      <c r="R115" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S115" s="3" t="s">
@@ -18211,7 +18208,7 @@
       <c r="Q116" s="66">
         <v>40</v>
       </c>
-      <c r="R116" s="67" t="s">
+      <c r="R116" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S116" s="3" t="s">
@@ -18291,7 +18288,7 @@
       <c r="Q117" s="66">
         <v>40</v>
       </c>
-      <c r="R117" s="67" t="s">
+      <c r="R117" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S117" s="3" t="s">
@@ -18359,7 +18356,7 @@
       <c r="Q118" s="66">
         <v>40</v>
       </c>
-      <c r="R118" s="67" t="s">
+      <c r="R118" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S118" s="3" t="s">
@@ -18443,7 +18440,7 @@
       <c r="Q119" s="66">
         <v>40</v>
       </c>
-      <c r="R119" s="67" t="s">
+      <c r="R119" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S119" s="3" t="s">
@@ -18513,7 +18510,7 @@
       <c r="Q120" s="66">
         <v>40</v>
       </c>
-      <c r="R120" s="67" t="s">
+      <c r="R120" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S120" s="3" t="s">
@@ -18603,7 +18600,7 @@
       <c r="Q121" s="66">
         <v>40</v>
       </c>
-      <c r="R121" s="67" t="s">
+      <c r="R121" s="3" t="s">
         <v>881</v>
       </c>
       <c r="S121" s="14" t="s">
@@ -18687,7 +18684,7 @@
       <c r="Q122" s="66">
         <v>40</v>
       </c>
-      <c r="R122" s="67" t="s">
+      <c r="R122" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S122" s="3" t="s">
@@ -18753,7 +18750,7 @@
       <c r="Q123" s="66">
         <v>40</v>
       </c>
-      <c r="R123" s="67" t="s">
+      <c r="R123" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S123" s="3" t="s">
@@ -18837,7 +18834,7 @@
       <c r="Q124" s="66">
         <v>40</v>
       </c>
-      <c r="R124" s="67" t="s">
+      <c r="R124" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S124" s="3" t="s">
@@ -18913,7 +18910,7 @@
       <c r="Q125" s="66">
         <v>40</v>
       </c>
-      <c r="R125" s="67" t="s">
+      <c r="R125" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S125" s="3" t="s">
@@ -18999,7 +18996,7 @@
       <c r="Q126" s="66">
         <v>40</v>
       </c>
-      <c r="R126" s="67" t="s">
+      <c r="R126" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S126" s="3" t="s">
@@ -19093,7 +19090,7 @@
       <c r="Q127" s="66">
         <v>40</v>
       </c>
-      <c r="R127" s="67" t="s">
+      <c r="R127" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S127" s="3" t="s">
@@ -19173,7 +19170,7 @@
       <c r="Q128" s="66">
         <v>40</v>
       </c>
-      <c r="R128" s="67" t="s">
+      <c r="R128" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S128" s="3" t="s">
@@ -19255,7 +19252,7 @@
       <c r="Q129" s="66">
         <v>40</v>
       </c>
-      <c r="R129" s="67" t="s">
+      <c r="R129" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S129" s="3" t="s">
@@ -19339,7 +19336,7 @@
       <c r="Q130" s="66">
         <v>40</v>
       </c>
-      <c r="R130" s="67" t="s">
+      <c r="R130" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S130" s="3" t="s">
@@ -19419,7 +19416,7 @@
       <c r="Q131" s="66">
         <v>40</v>
       </c>
-      <c r="R131" s="67" t="s">
+      <c r="R131" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S131" s="3" t="s">
@@ -19499,7 +19496,7 @@
       <c r="Q132" s="66">
         <v>40</v>
       </c>
-      <c r="R132" s="67" t="s">
+      <c r="R132" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S132" s="3" t="s">
@@ -19579,7 +19576,7 @@
       <c r="Q133" s="66">
         <v>40</v>
       </c>
-      <c r="R133" s="67" t="s">
+      <c r="R133" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S133" s="3" t="s">
@@ -19643,7 +19640,7 @@
       <c r="Q134" s="66">
         <v>73</v>
       </c>
-      <c r="R134" s="67" t="s">
+      <c r="R134" s="3" t="s">
         <v>313</v>
       </c>
       <c r="S134" s="12">
@@ -19725,7 +19722,7 @@
       <c r="Q135" s="66">
         <v>40</v>
       </c>
-      <c r="R135" s="67" t="s">
+      <c r="R135" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S135" s="3" t="s">
@@ -19813,7 +19810,7 @@
       <c r="Q136" s="66">
         <v>132</v>
       </c>
-      <c r="R136" s="67" t="s">
+      <c r="R136" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S136" s="3" t="s">
@@ -19895,7 +19892,7 @@
       <c r="Q137" s="66">
         <v>132</v>
       </c>
-      <c r="R137" s="67" t="s">
+      <c r="R137" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S137" s="3" t="s">
@@ -19963,7 +19960,7 @@
       <c r="Q138" s="66">
         <v>40</v>
       </c>
-      <c r="R138" s="67" t="s">
+      <c r="R138" s="3" t="s">
         <v>970</v>
       </c>
       <c r="S138" s="3" t="s">
@@ -20039,7 +20036,7 @@
       <c r="Q139" s="66">
         <v>40</v>
       </c>
-      <c r="R139" s="67" t="s">
+      <c r="R139" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S139" s="3" t="s">
@@ -20129,7 +20126,7 @@
       <c r="Q140" s="66">
         <v>40</v>
       </c>
-      <c r="R140" s="67" t="s">
+      <c r="R140" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S140" s="3" t="s">
@@ -20211,7 +20208,7 @@
       <c r="Q141" s="66">
         <v>40</v>
       </c>
-      <c r="R141" s="67" t="s">
+      <c r="R141" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S141" s="3" t="s">
@@ -20279,7 +20276,7 @@
       <c r="Q142" s="66">
         <v>40</v>
       </c>
-      <c r="R142" s="67" t="s">
+      <c r="R142" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S142" s="3" t="s">
@@ -20359,7 +20356,7 @@
       <c r="Q143" s="66">
         <v>40</v>
       </c>
-      <c r="R143" s="67" t="s">
+      <c r="R143" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S143" s="3" t="s">
@@ -20447,7 +20444,7 @@
       <c r="Q144" s="66">
         <v>40</v>
       </c>
-      <c r="R144" s="67" t="s">
+      <c r="R144" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S144" s="3" t="s">
@@ -20511,7 +20508,7 @@
       <c r="Q145" s="66">
         <v>40</v>
       </c>
-      <c r="R145" s="67" t="s">
+      <c r="R145" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S145" s="3" t="s">
@@ -20575,7 +20572,7 @@
       <c r="Q146" s="66">
         <v>43</v>
       </c>
-      <c r="R146" s="67" t="s">
+      <c r="R146" s="3" t="s">
         <v>313</v>
       </c>
       <c r="S146" s="12">
@@ -20657,7 +20654,7 @@
       <c r="Q147" s="66">
         <v>40</v>
       </c>
-      <c r="R147" s="67" t="s">
+      <c r="R147" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S147" s="3" t="s">
@@ -20727,7 +20724,7 @@
       <c r="Q148" s="66">
         <v>40</v>
       </c>
-      <c r="R148" s="67" t="s">
+      <c r="R148" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S148" s="3" t="s">
@@ -20813,7 +20810,7 @@
       <c r="Q149" s="66">
         <v>40</v>
       </c>
-      <c r="R149" s="67" t="s">
+      <c r="R149" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S149" s="3" t="s">
@@ -20893,7 +20890,7 @@
       <c r="Q150" s="66">
         <v>132</v>
       </c>
-      <c r="R150" s="67" t="s">
+      <c r="R150" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S150" s="3" t="s">
@@ -20961,7 +20958,7 @@
       <c r="Q151" s="66">
         <v>132</v>
       </c>
-      <c r="R151" s="67" t="s">
+      <c r="R151" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S151" s="3" t="s">
@@ -21017,7 +21014,7 @@
       <c r="Q152" s="66">
         <v>132</v>
       </c>
-      <c r="R152" s="67" t="s">
+      <c r="R152" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S152" s="3" t="s">
@@ -21073,7 +21070,7 @@
       <c r="Q153" s="66">
         <v>132</v>
       </c>
-      <c r="R153" s="67" t="s">
+      <c r="R153" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S153" s="3" t="s">
@@ -21129,7 +21126,7 @@
       <c r="Q154" s="66">
         <v>132</v>
       </c>
-      <c r="R154" s="67" t="s">
+      <c r="R154" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S154" s="3" t="s">
@@ -21191,7 +21188,7 @@
       <c r="Q155" s="66">
         <v>132</v>
       </c>
-      <c r="R155" s="67" t="s">
+      <c r="R155" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S155" s="3" t="s">
@@ -21251,7 +21248,7 @@
       <c r="Q156" s="66">
         <v>132</v>
       </c>
-      <c r="R156" s="67" t="s">
+      <c r="R156" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S156" s="3" t="s">
@@ -21319,7 +21316,7 @@
       <c r="Q157" s="66">
         <v>132</v>
       </c>
-      <c r="R157" s="67" t="s">
+      <c r="R157" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S157" s="3" t="s">
@@ -21381,7 +21378,7 @@
       <c r="Q158" s="66">
         <v>40</v>
       </c>
-      <c r="R158" s="67" t="s">
+      <c r="R158" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S158" s="3" t="s">
@@ -21463,7 +21460,7 @@
       <c r="Q159" s="66">
         <v>40</v>
       </c>
-      <c r="R159" s="67" t="s">
+      <c r="R159" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S159" s="3" t="s">
@@ -21539,7 +21536,7 @@
       <c r="Q160" s="66">
         <v>40</v>
       </c>
-      <c r="R160" s="67" t="s">
+      <c r="R160" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S160" s="3" t="s">
@@ -21623,7 +21620,7 @@
       <c r="Q161" s="66">
         <v>40</v>
       </c>
-      <c r="R161" s="67" t="s">
+      <c r="R161" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S161" s="3" t="s">
@@ -21713,7 +21710,7 @@
       <c r="Q162" s="66">
         <v>40</v>
       </c>
-      <c r="R162" s="67" t="s">
+      <c r="R162" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S162" s="3" t="s">
@@ -21793,7 +21790,7 @@
       <c r="Q163" s="66">
         <v>40</v>
       </c>
-      <c r="R163" s="67" t="s">
+      <c r="R163" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S163" s="3" t="s">
@@ -21879,7 +21876,7 @@
       <c r="Q164" s="66">
         <v>40</v>
       </c>
-      <c r="R164" s="67" t="s">
+      <c r="R164" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S164" s="3" t="s">
@@ -21945,7 +21942,7 @@
       <c r="Q165" s="66">
         <v>40</v>
       </c>
-      <c r="R165" s="67" t="s">
+      <c r="R165" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S165" s="3" t="s">
@@ -22009,7 +22006,7 @@
       <c r="Q166" s="66">
         <v>40</v>
       </c>
-      <c r="R166" s="67" t="s">
+      <c r="R166" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S166" s="3" t="s">
@@ -22095,7 +22092,7 @@
       <c r="Q167" s="66">
         <v>40</v>
       </c>
-      <c r="R167" s="67" t="s">
+      <c r="R167" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S167" s="3" t="s">
@@ -22179,7 +22176,7 @@
       <c r="Q168" s="66">
         <v>40</v>
       </c>
-      <c r="R168" s="67" t="s">
+      <c r="R168" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S168" s="3" t="s">
@@ -22263,7 +22260,7 @@
       <c r="Q169" s="66">
         <v>40</v>
       </c>
-      <c r="R169" s="67" t="s">
+      <c r="R169" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S169" s="3" t="s">
@@ -22355,7 +22352,7 @@
       <c r="Q170" s="66">
         <v>40</v>
       </c>
-      <c r="R170" s="67" t="s">
+      <c r="R170" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S170" s="3" t="s">
@@ -22445,7 +22442,7 @@
       <c r="Q171" s="66">
         <v>40</v>
       </c>
-      <c r="R171" s="67" t="s">
+      <c r="R171" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S171" s="3" t="s">
@@ -22529,7 +22526,7 @@
       <c r="Q172" s="66">
         <v>40</v>
       </c>
-      <c r="R172" s="67" t="s">
+      <c r="R172" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S172" s="3" t="s">
@@ -22611,7 +22608,7 @@
       <c r="Q173" s="66">
         <v>40</v>
       </c>
-      <c r="R173" s="67" t="s">
+      <c r="R173" s="3" t="s">
         <v>1132</v>
       </c>
       <c r="S173" s="3" t="s">
@@ -22685,7 +22682,7 @@
       <c r="Q174" s="66">
         <v>40</v>
       </c>
-      <c r="R174" s="67" t="s">
+      <c r="R174" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S174" s="3" t="s">
@@ -22771,7 +22768,7 @@
       <c r="Q175" s="66">
         <v>40</v>
       </c>
-      <c r="R175" s="67" t="s">
+      <c r="R175" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S175" s="3" t="s">
@@ -22863,7 +22860,7 @@
       <c r="Q176" s="66">
         <v>40</v>
       </c>
-      <c r="R176" s="67" t="s">
+      <c r="R176" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S176" s="3" t="s">
@@ -22951,7 +22948,7 @@
       <c r="Q177" s="66">
         <v>40</v>
       </c>
-      <c r="R177" s="67" t="s">
+      <c r="R177" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S177" s="3" t="s">
@@ -23041,7 +23038,7 @@
       <c r="Q178" s="66">
         <v>40</v>
       </c>
-      <c r="R178" s="67" t="s">
+      <c r="R178" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S178" s="3" t="s">
@@ -23133,7 +23130,7 @@
       <c r="Q179" s="66">
         <v>40</v>
       </c>
-      <c r="R179" s="67" t="s">
+      <c r="R179" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S179" s="3" t="s">
@@ -23219,7 +23216,7 @@
       <c r="Q180" s="66">
         <v>40</v>
       </c>
-      <c r="R180" s="67" t="s">
+      <c r="R180" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S180" s="3" t="s">
@@ -23311,7 +23308,7 @@
       <c r="Q181" s="66">
         <v>40</v>
       </c>
-      <c r="R181" s="67" t="s">
+      <c r="R181" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S181" s="3" t="s">
@@ -23391,7 +23388,7 @@
       <c r="Q182" s="66">
         <v>132</v>
       </c>
-      <c r="R182" s="67" t="s">
+      <c r="R182" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S182" s="3" t="s">
@@ -23455,7 +23452,7 @@
       <c r="Q183" s="66">
         <v>40</v>
       </c>
-      <c r="R183" s="67" t="s">
+      <c r="R183" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S183" s="3" t="s">
@@ -23523,7 +23520,7 @@
       <c r="Q184" s="66">
         <v>132</v>
       </c>
-      <c r="R184" s="67" t="s">
+      <c r="R184" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S184" s="3" t="s">
@@ -23589,7 +23586,7 @@
       <c r="Q185" s="66">
         <v>132</v>
       </c>
-      <c r="R185" s="67" t="s">
+      <c r="R185" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S185" s="3" t="s">
@@ -23661,7 +23658,7 @@
       <c r="Q186" s="66">
         <v>132</v>
       </c>
-      <c r="R186" s="67" t="s">
+      <c r="R186" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S186" s="3" t="s">
@@ -23741,7 +23738,7 @@
       <c r="Q187" s="66">
         <v>132</v>
       </c>
-      <c r="R187" s="67" t="s">
+      <c r="R187" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S187" s="3" t="s">
@@ -23823,11 +23820,11 @@
       <c r="Q188" s="66">
         <v>122</v>
       </c>
-      <c r="R188" s="67">
-        <v>22122</v>
-      </c>
-      <c r="S188" s="12">
-        <v>106107</v>
+      <c r="R188" s="14" t="s">
+        <v>2637</v>
+      </c>
+      <c r="S188" s="14" t="s">
+        <v>683</v>
       </c>
       <c r="T188" s="16" t="s">
         <v>684</v>
@@ -23887,7 +23884,7 @@
       <c r="Q189" s="66">
         <v>40</v>
       </c>
-      <c r="R189" s="67" t="s">
+      <c r="R189" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S189" s="3" t="s">
@@ -23951,7 +23948,7 @@
       <c r="Q190" s="66">
         <v>40</v>
       </c>
-      <c r="R190" s="67" t="s">
+      <c r="R190" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S190" s="3" t="s">
@@ -24019,7 +24016,7 @@
       <c r="Q191" s="66">
         <v>132</v>
       </c>
-      <c r="R191" s="67" t="s">
+      <c r="R191" s="3" t="s">
         <v>1226</v>
       </c>
       <c r="S191" s="3" t="s">
@@ -24105,7 +24102,7 @@
       <c r="Q192" s="66">
         <v>40</v>
       </c>
-      <c r="R192" s="67" t="s">
+      <c r="R192" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S192" s="3" t="s">
@@ -24193,7 +24190,7 @@
       <c r="Q193" s="66">
         <v>40</v>
       </c>
-      <c r="R193" s="67" t="s">
+      <c r="R193" s="3" t="s">
         <v>1241</v>
       </c>
       <c r="S193" s="14" t="s">
@@ -24265,11 +24262,11 @@
       <c r="Q194" s="66">
         <v>73</v>
       </c>
-      <c r="R194" s="70" t="s">
+      <c r="R194" s="67" t="s">
         <v>313</v>
       </c>
-      <c r="S194" s="65">
-        <v>2488100</v>
+      <c r="S194" s="68" t="s">
+        <v>1937</v>
       </c>
       <c r="T194" s="62" t="s">
         <v>374</v>
@@ -24351,7 +24348,7 @@
       <c r="Q195" s="66">
         <v>40</v>
       </c>
-      <c r="R195" s="67" t="s">
+      <c r="R195" s="3" t="s">
         <v>421</v>
       </c>
       <c r="S195" s="3" t="s">
@@ -24437,7 +24434,7 @@
       <c r="Q196" s="66">
         <v>40</v>
       </c>
-      <c r="R196" s="67" t="s">
+      <c r="R196" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S196" s="3" t="s">
@@ -24517,7 +24514,7 @@
       <c r="Q197" s="66">
         <v>40</v>
       </c>
-      <c r="R197" s="67" t="s">
+      <c r="R197" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S197" s="3" t="s">
@@ -24591,7 +24588,7 @@
       <c r="Q198" s="66">
         <v>40</v>
       </c>
-      <c r="R198" s="67" t="s">
+      <c r="R198" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S198" s="3" t="s">
@@ -24653,11 +24650,11 @@
       <c r="Q199" s="66">
         <v>122</v>
       </c>
-      <c r="R199" s="67">
-        <v>22122</v>
-      </c>
-      <c r="S199" s="12">
-        <v>106107</v>
+      <c r="R199" s="14" t="s">
+        <v>2637</v>
+      </c>
+      <c r="S199" s="14" t="s">
+        <v>683</v>
       </c>
       <c r="T199" s="16" t="s">
         <v>684</v>
@@ -24725,7 +24722,7 @@
       <c r="Q200" s="66">
         <v>40</v>
       </c>
-      <c r="R200" s="67" t="s">
+      <c r="R200" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S200" s="3" t="s">
@@ -24801,7 +24798,7 @@
       <c r="Q201" s="66">
         <v>40</v>
       </c>
-      <c r="R201" s="67" t="s">
+      <c r="R201" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S201" s="3" t="s">
@@ -24873,7 +24870,7 @@
       <c r="Q202" s="66">
         <v>40</v>
       </c>
-      <c r="R202" s="67" t="s">
+      <c r="R202" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S202" s="3" t="s">
@@ -24963,7 +24960,7 @@
       <c r="Q203" s="66">
         <v>40</v>
       </c>
-      <c r="R203" s="67" t="s">
+      <c r="R203" s="3" t="s">
         <v>1304</v>
       </c>
       <c r="S203" s="14" t="s">
@@ -25037,11 +25034,11 @@
       <c r="Q204" s="66">
         <v>122</v>
       </c>
-      <c r="R204" s="67">
-        <v>22122</v>
-      </c>
-      <c r="S204" s="12">
-        <v>106107</v>
+      <c r="R204" s="14" t="s">
+        <v>2637</v>
+      </c>
+      <c r="S204" s="14" t="s">
+        <v>683</v>
       </c>
       <c r="T204" s="13" t="s">
         <v>684</v>
@@ -25107,7 +25104,7 @@
       <c r="Q205" s="66">
         <v>40</v>
       </c>
-      <c r="R205" s="67" t="s">
+      <c r="R205" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S205" s="3" t="s">
@@ -25169,7 +25166,7 @@
       <c r="Q206" s="66">
         <v>132</v>
       </c>
-      <c r="R206" s="67" t="s">
+      <c r="R206" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S206" s="3" t="s">
@@ -25243,7 +25240,7 @@
       <c r="Q207" s="66">
         <v>40</v>
       </c>
-      <c r="R207" s="67" t="s">
+      <c r="R207" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S207" s="3" t="s">
@@ -25313,7 +25310,7 @@
       <c r="Q208" s="66">
         <v>40</v>
       </c>
-      <c r="R208" s="67" t="s">
+      <c r="R208" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S208" s="3" t="s">
@@ -25385,7 +25382,7 @@
       <c r="Q209" s="66">
         <v>40</v>
       </c>
-      <c r="R209" s="67" t="s">
+      <c r="R209" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S209" s="3" t="s">
@@ -25469,7 +25466,7 @@
       <c r="Q210" s="66">
         <v>40</v>
       </c>
-      <c r="R210" s="67" t="s">
+      <c r="R210" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S210" s="3" t="s">
@@ -25557,7 +25554,7 @@
       <c r="Q211" s="66">
         <v>40</v>
       </c>
-      <c r="R211" s="67" t="s">
+      <c r="R211" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S211" s="3" t="s">
@@ -25643,7 +25640,7 @@
       <c r="Q212" s="66">
         <v>40</v>
       </c>
-      <c r="R212" s="67" t="s">
+      <c r="R212" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S212" s="3" t="s">
@@ -25723,7 +25720,7 @@
       <c r="Q213" s="66">
         <v>40</v>
       </c>
-      <c r="R213" s="67" t="s">
+      <c r="R213" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S213" s="14" t="s">
@@ -25809,7 +25806,7 @@
       <c r="Q214" s="66">
         <v>40</v>
       </c>
-      <c r="R214" s="67" t="s">
+      <c r="R214" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S214" s="3" t="s">
@@ -25897,7 +25894,7 @@
       <c r="Q215" s="66">
         <v>40</v>
       </c>
-      <c r="R215" s="67" t="s">
+      <c r="R215" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S215" s="3" t="s">
@@ -25977,7 +25974,7 @@
       <c r="Q216" s="66">
         <v>40</v>
       </c>
-      <c r="R216" s="67" t="s">
+      <c r="R216" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S216" s="3" t="s">
@@ -26049,7 +26046,7 @@
       <c r="Q217" s="66">
         <v>40</v>
       </c>
-      <c r="R217" s="67" t="s">
+      <c r="R217" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S217" s="3" t="s">
@@ -26137,7 +26134,7 @@
       <c r="Q218" s="66">
         <v>40</v>
       </c>
-      <c r="R218" s="67" t="s">
+      <c r="R218" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S218" s="3" t="s">
@@ -26221,7 +26218,7 @@
       <c r="Q219" s="66">
         <v>132</v>
       </c>
-      <c r="R219" s="67" t="s">
+      <c r="R219" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S219" s="3" t="s">
@@ -26303,11 +26300,11 @@
       <c r="Q220" s="66">
         <v>40</v>
       </c>
-      <c r="R220" s="67" t="s">
+      <c r="R220" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S220" s="12">
-        <v>24100</v>
+      <c r="S220" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T220" s="13" t="s">
         <v>374</v>
@@ -26391,7 +26388,7 @@
       <c r="Q221" s="66">
         <v>40</v>
       </c>
-      <c r="R221" s="67" t="s">
+      <c r="R221" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S221" s="3" t="s">
@@ -26471,7 +26468,7 @@
       <c r="Q222" s="66">
         <v>40</v>
       </c>
-      <c r="R222" s="67" t="s">
+      <c r="R222" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S222" s="14" t="s">
@@ -26543,7 +26540,7 @@
       <c r="Q223" s="66">
         <v>40</v>
       </c>
-      <c r="R223" s="67" t="s">
+      <c r="R223" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S223" s="3" t="s">
@@ -26623,11 +26620,11 @@
       <c r="Q224" s="66">
         <v>122</v>
       </c>
-      <c r="R224" s="67">
-        <v>22122</v>
-      </c>
-      <c r="S224" s="12">
-        <v>106107</v>
+      <c r="R224" s="14" t="s">
+        <v>2637</v>
+      </c>
+      <c r="S224" s="14" t="s">
+        <v>683</v>
       </c>
       <c r="T224" s="13" t="s">
         <v>684</v>
@@ -26687,7 +26684,7 @@
       <c r="Q225" s="66">
         <v>40</v>
       </c>
-      <c r="R225" s="67" t="s">
+      <c r="R225" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S225" s="3" t="s">
@@ -26769,7 +26766,7 @@
       <c r="Q226" s="66">
         <v>40</v>
       </c>
-      <c r="R226" s="67" t="s">
+      <c r="R226" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S226" s="3" t="s">
@@ -26837,7 +26834,7 @@
       <c r="Q227" s="66">
         <v>40</v>
       </c>
-      <c r="R227" s="67" t="s">
+      <c r="R227" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S227" s="3" t="s">
@@ -26903,7 +26900,7 @@
       <c r="Q228" s="66">
         <v>40</v>
       </c>
-      <c r="R228" s="67" t="s">
+      <c r="R228" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S228" s="3" t="s">
@@ -26973,7 +26970,7 @@
       <c r="Q229" s="66">
         <v>40</v>
       </c>
-      <c r="R229" s="67" t="s">
+      <c r="R229" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S229" s="3" t="s">
@@ -27039,7 +27036,7 @@
       <c r="Q230" s="66">
         <v>40</v>
       </c>
-      <c r="R230" s="67" t="s">
+      <c r="R230" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S230" s="3" t="s">
@@ -27113,7 +27110,7 @@
       <c r="Q231" s="66">
         <v>40</v>
       </c>
-      <c r="R231" s="67" t="s">
+      <c r="R231" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S231" s="3" t="s">
@@ -27199,7 +27196,7 @@
       <c r="Q232" s="66">
         <v>40</v>
       </c>
-      <c r="R232" s="67" t="s">
+      <c r="R232" s="3" t="s">
         <v>508</v>
       </c>
       <c r="S232" s="3" t="s">
@@ -27263,7 +27260,7 @@
       <c r="Q233" s="66">
         <v>40</v>
       </c>
-      <c r="R233" s="67" t="s">
+      <c r="R233" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S233" s="3" t="s">
@@ -27343,11 +27340,11 @@
       <c r="Q234" s="66">
         <v>122</v>
       </c>
-      <c r="R234" s="67">
-        <v>22122</v>
-      </c>
-      <c r="S234" s="12">
-        <v>106107</v>
+      <c r="R234" s="14" t="s">
+        <v>2637</v>
+      </c>
+      <c r="S234" s="14" t="s">
+        <v>683</v>
       </c>
       <c r="T234" s="16" t="s">
         <v>684</v>
@@ -27413,7 +27410,7 @@
       <c r="Q235" s="66">
         <v>40</v>
       </c>
-      <c r="R235" s="67" t="s">
+      <c r="R235" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S235" s="3" t="s">
@@ -27479,7 +27476,7 @@
       <c r="Q236" s="66">
         <v>40</v>
       </c>
-      <c r="R236" s="67" t="s">
+      <c r="R236" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S236" s="14" t="s">
@@ -27543,7 +27540,7 @@
       <c r="Q237" s="66">
         <v>40</v>
       </c>
-      <c r="R237" s="67" t="s">
+      <c r="R237" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S237" s="3" t="s">
@@ -27623,7 +27620,7 @@
       <c r="Q238" s="66">
         <v>40</v>
       </c>
-      <c r="R238" s="67" t="s">
+      <c r="R238" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S238" s="3" t="s">
@@ -27693,7 +27690,7 @@
       <c r="Q239" s="66">
         <v>40</v>
       </c>
-      <c r="R239" s="67" t="s">
+      <c r="R239" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S239" s="3" t="s">
@@ -27777,7 +27774,7 @@
       <c r="Q240" s="66">
         <v>40</v>
       </c>
-      <c r="R240" s="67" t="s">
+      <c r="R240" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S240" s="3" t="s">
@@ -27857,7 +27854,7 @@
       <c r="Q241" s="66">
         <v>40</v>
       </c>
-      <c r="R241" s="67" t="s">
+      <c r="R241" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S241" s="3" t="s">
@@ -27931,7 +27928,7 @@
       <c r="Q242" s="66">
         <v>40</v>
       </c>
-      <c r="R242" s="67" t="s">
+      <c r="R242" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S242" s="3" t="s">
@@ -27999,7 +27996,7 @@
       <c r="Q243" s="66">
         <v>40</v>
       </c>
-      <c r="R243" s="67" t="s">
+      <c r="R243" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S243" s="14" t="s">
@@ -28063,7 +28060,7 @@
       <c r="Q244" s="66">
         <v>40</v>
       </c>
-      <c r="R244" s="67" t="s">
+      <c r="R244" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S244" s="3" t="s">
@@ -28135,7 +28132,7 @@
       <c r="Q245" s="66">
         <v>40</v>
       </c>
-      <c r="R245" s="67" t="s">
+      <c r="R245" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S245" s="3" t="s">
@@ -28201,7 +28198,7 @@
       <c r="Q246" s="66">
         <v>40</v>
       </c>
-      <c r="R246" s="67" t="s">
+      <c r="R246" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S246" s="3" t="s">
@@ -28265,7 +28262,7 @@
       <c r="Q247" s="66">
         <v>40</v>
       </c>
-      <c r="R247" s="67" t="s">
+      <c r="R247" s="3" t="s">
         <v>274</v>
       </c>
       <c r="S247" s="14" t="s">
@@ -28353,11 +28350,11 @@
       <c r="Q248" s="66">
         <v>73</v>
       </c>
-      <c r="R248" s="67" t="s">
+      <c r="R248" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S248" s="12">
-        <v>24100</v>
+      <c r="S248" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T248" s="13" t="s">
         <v>374</v>
@@ -28443,7 +28440,7 @@
       <c r="Q249" s="66">
         <v>40</v>
       </c>
-      <c r="R249" s="67" t="s">
+      <c r="R249" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S249" s="3" t="s">
@@ -28537,7 +28534,7 @@
       <c r="Q250" s="66">
         <v>40</v>
       </c>
-      <c r="R250" s="67" t="s">
+      <c r="R250" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S250" s="3" t="s">
@@ -28619,7 +28616,7 @@
       <c r="Q251" s="66">
         <v>40</v>
       </c>
-      <c r="R251" s="67" t="s">
+      <c r="R251" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S251" s="3" t="s">
@@ -28689,7 +28686,7 @@
       <c r="Q252" s="66">
         <v>132</v>
       </c>
-      <c r="R252" s="67" t="s">
+      <c r="R252" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S252" s="3" t="s">
@@ -28765,7 +28762,7 @@
       <c r="Q253" s="66">
         <v>40</v>
       </c>
-      <c r="R253" s="67" t="s">
+      <c r="R253" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S253" s="3" t="s">
@@ -28837,7 +28834,7 @@
       <c r="Q254" s="66">
         <v>40</v>
       </c>
-      <c r="R254" s="67" t="s">
+      <c r="R254" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S254" s="3" t="s">
@@ -28923,7 +28920,7 @@
       <c r="Q255" s="66">
         <v>40</v>
       </c>
-      <c r="R255" s="67" t="s">
+      <c r="R255" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S255" s="3" t="s">
@@ -28997,7 +28994,7 @@
       <c r="Q256" s="66">
         <v>132</v>
       </c>
-      <c r="R256" s="67" t="s">
+      <c r="R256" s="3" t="s">
         <v>1572</v>
       </c>
       <c r="S256" s="3" t="s">
@@ -29083,7 +29080,7 @@
       <c r="Q257" s="66">
         <v>40</v>
       </c>
-      <c r="R257" s="67" t="s">
+      <c r="R257" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S257" s="3" t="s">
@@ -29171,7 +29168,7 @@
       <c r="Q258" s="66">
         <v>40</v>
       </c>
-      <c r="R258" s="67" t="s">
+      <c r="R258" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S258" s="3" t="s">
@@ -29253,7 +29250,7 @@
       <c r="Q259" s="66">
         <v>40</v>
       </c>
-      <c r="R259" s="67" t="s">
+      <c r="R259" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S259" s="3" t="s">
@@ -29331,7 +29328,7 @@
       <c r="Q260" s="66">
         <v>40</v>
       </c>
-      <c r="R260" s="67" t="s">
+      <c r="R260" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S260" s="3" t="s">
@@ -29425,7 +29422,7 @@
       <c r="Q261" s="66">
         <v>40</v>
       </c>
-      <c r="R261" s="67" t="s">
+      <c r="R261" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S261" s="3" t="s">
@@ -29511,7 +29508,7 @@
       <c r="Q262" s="66">
         <v>40</v>
       </c>
-      <c r="R262" s="67" t="s">
+      <c r="R262" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S262" s="3" t="s">
@@ -29605,7 +29602,7 @@
       <c r="Q263" s="66">
         <v>40</v>
       </c>
-      <c r="R263" s="67" t="s">
+      <c r="R263" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S263" s="3" t="s">
@@ -29687,7 +29684,7 @@
       <c r="Q264" s="66">
         <v>40</v>
       </c>
-      <c r="R264" s="67" t="s">
+      <c r="R264" s="3" t="s">
         <v>267</v>
       </c>
       <c r="S264" s="3" t="s">
@@ -29771,7 +29768,7 @@
       <c r="Q265" s="66">
         <v>40</v>
       </c>
-      <c r="R265" s="67" t="s">
+      <c r="R265" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S265" s="3" t="s">
@@ -29841,7 +29838,7 @@
       <c r="Q266" s="66">
         <v>40</v>
       </c>
-      <c r="R266" s="67" t="s">
+      <c r="R266" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S266" s="3" t="s">
@@ -29929,7 +29926,7 @@
       <c r="Q267" s="66">
         <v>40</v>
       </c>
-      <c r="R267" s="67" t="s">
+      <c r="R267" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S267" s="3" t="s">
@@ -30001,7 +29998,7 @@
       <c r="Q268" s="66">
         <v>40</v>
       </c>
-      <c r="R268" s="67" t="s">
+      <c r="R268" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S268" s="3" t="s">
@@ -30083,7 +30080,7 @@
       <c r="Q269" s="66">
         <v>40</v>
       </c>
-      <c r="R269" s="67" t="s">
+      <c r="R269" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S269" s="3" t="s">
@@ -30157,7 +30154,7 @@
       <c r="Q270" s="66">
         <v>40</v>
       </c>
-      <c r="R270" s="67" t="s">
+      <c r="R270" s="3" t="s">
         <v>1645</v>
       </c>
       <c r="S270" s="3" t="s">
@@ -30231,7 +30228,7 @@
       <c r="Q271" s="66">
         <v>40</v>
       </c>
-      <c r="R271" s="67" t="s">
+      <c r="R271" s="3" t="s">
         <v>421</v>
       </c>
       <c r="S271" s="3" t="s">
@@ -30311,7 +30308,7 @@
       <c r="Q272" s="66">
         <v>40</v>
       </c>
-      <c r="R272" s="67" t="s">
+      <c r="R272" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S272" s="3" t="s">
@@ -30401,7 +30398,7 @@
       <c r="Q273" s="66">
         <v>40</v>
       </c>
-      <c r="R273" s="67" t="s">
+      <c r="R273" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S273" s="3" t="s">
@@ -30481,7 +30478,7 @@
       <c r="Q274" s="66">
         <v>40</v>
       </c>
-      <c r="R274" s="67" t="s">
+      <c r="R274" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S274" s="3" t="s">
@@ -30549,7 +30546,7 @@
       <c r="Q275" s="66">
         <v>40</v>
       </c>
-      <c r="R275" s="67" t="s">
+      <c r="R275" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S275" s="3" t="s">
@@ -30635,7 +30632,7 @@
       <c r="Q276" s="66">
         <v>40</v>
       </c>
-      <c r="R276" s="67" t="s">
+      <c r="R276" s="3" t="s">
         <v>508</v>
       </c>
       <c r="S276" s="3" t="s">
@@ -30703,7 +30700,7 @@
       <c r="Q277" s="66">
         <v>40</v>
       </c>
-      <c r="R277" s="67" t="s">
+      <c r="R277" s="3" t="s">
         <v>274</v>
       </c>
       <c r="S277" s="14" t="s">
@@ -30785,7 +30782,7 @@
       <c r="Q278" s="66">
         <v>40</v>
       </c>
-      <c r="R278" s="67" t="s">
+      <c r="R278" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S278" s="3" t="s">
@@ -30869,7 +30866,7 @@
       <c r="Q279" s="66">
         <v>40</v>
       </c>
-      <c r="R279" s="67" t="s">
+      <c r="R279" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S279" s="3" t="s">
@@ -30937,7 +30934,7 @@
       <c r="Q280" s="66">
         <v>40</v>
       </c>
-      <c r="R280" s="67" t="s">
+      <c r="R280" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S280" s="3" t="s">
@@ -31017,7 +31014,7 @@
       <c r="Q281" s="66">
         <v>40</v>
       </c>
-      <c r="R281" s="67" t="s">
+      <c r="R281" s="3" t="s">
         <v>970</v>
       </c>
       <c r="S281" s="3" t="s">
@@ -31091,7 +31088,7 @@
       <c r="Q282" s="66">
         <v>40</v>
       </c>
-      <c r="R282" s="67" t="s">
+      <c r="R282" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S282" s="3" t="s">
@@ -31177,7 +31174,7 @@
       <c r="Q283" s="66">
         <v>40</v>
       </c>
-      <c r="R283" s="67" t="s">
+      <c r="R283" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S283" s="3" t="s">
@@ -31259,7 +31256,7 @@
       <c r="Q284" s="66">
         <v>40</v>
       </c>
-      <c r="R284" s="67" t="s">
+      <c r="R284" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S284" s="3" t="s">
@@ -31347,7 +31344,7 @@
       <c r="Q285" s="66">
         <v>40</v>
       </c>
-      <c r="R285" s="67" t="s">
+      <c r="R285" s="3" t="s">
         <v>1734</v>
       </c>
       <c r="S285" s="3" t="s">
@@ -31421,7 +31418,7 @@
       <c r="Q286" s="66">
         <v>40</v>
       </c>
-      <c r="R286" s="67" t="s">
+      <c r="R286" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S286" s="3" t="s">
@@ -31507,7 +31504,7 @@
       <c r="Q287" s="66">
         <v>40</v>
       </c>
-      <c r="R287" s="67" t="s">
+      <c r="R287" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S287" s="3" t="s">
@@ -31595,7 +31592,7 @@
       <c r="Q288" s="66">
         <v>73</v>
       </c>
-      <c r="R288" s="67" t="s">
+      <c r="R288" s="3" t="s">
         <v>313</v>
       </c>
       <c r="S288" s="14" t="s">
@@ -31683,7 +31680,7 @@
       <c r="Q289" s="66">
         <v>132</v>
       </c>
-      <c r="R289" s="67" t="s">
+      <c r="R289" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S289" s="3" t="s">
@@ -31769,7 +31766,7 @@
       <c r="Q290" s="66">
         <v>40</v>
       </c>
-      <c r="R290" s="67" t="s">
+      <c r="R290" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S290" s="3" t="s">
@@ -31845,7 +31842,7 @@
       <c r="Q291" s="66">
         <v>40</v>
       </c>
-      <c r="R291" s="67" t="s">
+      <c r="R291" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S291" s="3" t="s">
@@ -31919,7 +31916,7 @@
       <c r="Q292" s="66">
         <v>40</v>
       </c>
-      <c r="R292" s="67" t="s">
+      <c r="R292" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S292" s="3" t="s">
@@ -31995,7 +31992,7 @@
       <c r="Q293" s="66">
         <v>132</v>
       </c>
-      <c r="R293" s="67" t="s">
+      <c r="R293" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S293" s="3" t="s">
@@ -32067,7 +32064,7 @@
       <c r="Q294" s="66">
         <v>40</v>
       </c>
-      <c r="R294" s="67" t="s">
+      <c r="R294" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S294" s="3" t="s">
@@ -32135,7 +32132,7 @@
       <c r="Q295" s="66">
         <v>40</v>
       </c>
-      <c r="R295" s="67" t="s">
+      <c r="R295" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S295" s="3" t="s">
@@ -32229,7 +32226,7 @@
       <c r="Q296" s="66">
         <v>73</v>
       </c>
-      <c r="R296" s="67" t="s">
+      <c r="R296" s="3" t="s">
         <v>313</v>
       </c>
       <c r="S296" s="12">
@@ -32309,7 +32306,7 @@
       <c r="Q297" s="66">
         <v>40</v>
       </c>
-      <c r="R297" s="67" t="s">
+      <c r="R297" s="3" t="s">
         <v>1734</v>
       </c>
       <c r="S297" s="3" t="s">
@@ -32385,7 +32382,7 @@
       <c r="Q298" s="66">
         <v>40</v>
       </c>
-      <c r="R298" s="67" t="s">
+      <c r="R298" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S298" s="3" t="s">
@@ -32471,7 +32468,7 @@
       <c r="Q299" s="66">
         <v>40</v>
       </c>
-      <c r="R299" s="67" t="s">
+      <c r="R299" s="3" t="s">
         <v>1734</v>
       </c>
       <c r="S299" s="3" t="s">
@@ -32547,7 +32544,7 @@
       <c r="Q300" s="66">
         <v>40</v>
       </c>
-      <c r="R300" s="67" t="s">
+      <c r="R300" s="3" t="s">
         <v>1734</v>
       </c>
       <c r="S300" s="3" t="s">
@@ -32623,7 +32620,7 @@
       <c r="Q301" s="66">
         <v>40</v>
       </c>
-      <c r="R301" s="67" t="s">
+      <c r="R301" s="3" t="s">
         <v>1734</v>
       </c>
       <c r="S301" s="3" t="s">
@@ -32701,7 +32698,7 @@
       <c r="Q302" s="66">
         <v>40</v>
       </c>
-      <c r="R302" s="67" t="s">
+      <c r="R302" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S302" s="3" t="s">
@@ -32769,7 +32766,7 @@
       <c r="Q303" s="66">
         <v>40</v>
       </c>
-      <c r="R303" s="67" t="s">
+      <c r="R303" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S303" s="3" t="s">
@@ -32851,7 +32848,7 @@
       <c r="Q304" s="66">
         <v>40</v>
       </c>
-      <c r="R304" s="67" t="s">
+      <c r="R304" s="3" t="s">
         <v>267</v>
       </c>
       <c r="S304" s="3" t="s">
@@ -32941,7 +32938,7 @@
       <c r="Q305" s="66">
         <v>40</v>
       </c>
-      <c r="R305" s="67" t="s">
+      <c r="R305" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S305" s="3" t="s">
@@ -33025,7 +33022,7 @@
       <c r="Q306" s="66">
         <v>40</v>
       </c>
-      <c r="R306" s="67" t="s">
+      <c r="R306" s="3" t="s">
         <v>1734</v>
       </c>
       <c r="S306" s="3" t="s">
@@ -33099,7 +33096,7 @@
       <c r="Q307" s="66">
         <v>40</v>
       </c>
-      <c r="R307" s="67" t="s">
+      <c r="R307" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S307" s="3" t="s">
@@ -33187,7 +33184,7 @@
       <c r="Q308" s="66">
         <v>132</v>
       </c>
-      <c r="R308" s="67" t="s">
+      <c r="R308" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S308" s="14" t="s">
@@ -33277,7 +33274,7 @@
       <c r="Q309" s="66">
         <v>40</v>
       </c>
-      <c r="R309" s="67" t="s">
+      <c r="R309" s="3" t="s">
         <v>454</v>
       </c>
       <c r="S309" s="14" t="s">
@@ -33367,7 +33364,7 @@
       <c r="Q310" s="66">
         <v>40</v>
       </c>
-      <c r="R310" s="67" t="s">
+      <c r="R310" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S310" s="3" t="s">
@@ -33455,7 +33452,7 @@
       <c r="Q311" s="66">
         <v>40</v>
       </c>
-      <c r="R311" s="67" t="s">
+      <c r="R311" s="3" t="s">
         <v>1877</v>
       </c>
       <c r="S311" s="3" t="s">
@@ -33547,7 +33544,7 @@
       <c r="Q312" s="66">
         <v>40</v>
       </c>
-      <c r="R312" s="67" t="s">
+      <c r="R312" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S312" s="3" t="s">
@@ -33631,7 +33628,7 @@
       <c r="Q313" s="66">
         <v>40</v>
       </c>
-      <c r="R313" s="67" t="s">
+      <c r="R313" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S313" s="3" t="s">
@@ -33713,7 +33710,7 @@
       <c r="Q314" s="66">
         <v>40</v>
       </c>
-      <c r="R314" s="67" t="s">
+      <c r="R314" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S314" s="3" t="s">
@@ -33795,7 +33792,7 @@
       <c r="Q315" s="66">
         <v>40</v>
       </c>
-      <c r="R315" s="67" t="s">
+      <c r="R315" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S315" s="3" t="s">
@@ -33881,11 +33878,11 @@
       <c r="Q316" s="66">
         <v>73</v>
       </c>
-      <c r="R316" s="67" t="s">
+      <c r="R316" s="3" t="s">
         <v>1898</v>
       </c>
-      <c r="S316" s="12">
-        <v>24100</v>
+      <c r="S316" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T316" s="13" t="s">
         <v>1899</v>
@@ -33969,7 +33966,7 @@
       <c r="Q317" s="66">
         <v>40</v>
       </c>
-      <c r="R317" s="67" t="s">
+      <c r="R317" s="3" t="s">
         <v>1905</v>
       </c>
       <c r="S317" s="3" t="s">
@@ -34059,7 +34056,7 @@
       <c r="Q318" s="66">
         <v>40</v>
       </c>
-      <c r="R318" s="67" t="s">
+      <c r="R318" s="3" t="s">
         <v>1905</v>
       </c>
       <c r="S318" s="3" t="s">
@@ -34145,7 +34142,7 @@
       <c r="Q319" s="66">
         <v>40</v>
       </c>
-      <c r="R319" s="67" t="s">
+      <c r="R319" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S319" s="3" t="s">
@@ -34235,7 +34232,7 @@
       <c r="Q320" s="66">
         <v>40</v>
       </c>
-      <c r="R320" s="67" t="s">
+      <c r="R320" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S320" s="3" t="s">
@@ -34309,7 +34306,7 @@
       <c r="Q321" s="66">
         <v>40</v>
       </c>
-      <c r="R321" s="67" t="s">
+      <c r="R321" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S321" s="3" t="s">
@@ -34393,7 +34390,7 @@
       <c r="Q322" s="66">
         <v>43</v>
       </c>
-      <c r="R322" s="71" t="s">
+      <c r="R322" s="18" t="s">
         <v>1936</v>
       </c>
       <c r="S322" s="19" t="s">
@@ -34477,7 +34474,7 @@
       <c r="Q323" s="66">
         <v>40</v>
       </c>
-      <c r="R323" s="67" t="s">
+      <c r="R323" s="3" t="s">
         <v>1905</v>
       </c>
       <c r="S323" s="3" t="s">
@@ -34561,7 +34558,7 @@
       <c r="Q324" s="66">
         <v>40</v>
       </c>
-      <c r="R324" s="67" t="s">
+      <c r="R324" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S324" s="3" t="s">
@@ -34639,7 +34636,7 @@
       <c r="Q325" s="66">
         <v>40</v>
       </c>
-      <c r="R325" s="67" t="s">
+      <c r="R325" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S325" s="3" t="s">
@@ -34707,7 +34704,7 @@
       <c r="Q326" s="66">
         <v>40</v>
       </c>
-      <c r="R326" s="67" t="s">
+      <c r="R326" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S326" s="3" t="s">
@@ -34789,7 +34786,7 @@
       <c r="Q327" s="66">
         <v>132</v>
       </c>
-      <c r="R327" s="67" t="s">
+      <c r="R327" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S327" s="3" t="s">
@@ -34861,7 +34858,7 @@
       <c r="Q328" s="66">
         <v>40</v>
       </c>
-      <c r="R328" s="67" t="s">
+      <c r="R328" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S328" s="3" t="s">
@@ -34925,7 +34922,7 @@
       <c r="Q329" s="66">
         <v>40</v>
       </c>
-      <c r="R329" s="67" t="s">
+      <c r="R329" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S329" s="3" t="s">
@@ -34995,7 +34992,7 @@
       <c r="Q330" s="66">
         <v>40</v>
       </c>
-      <c r="R330" s="67" t="s">
+      <c r="R330" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S330" s="3" t="s">
@@ -35073,7 +35070,7 @@
       <c r="Q331" s="66">
         <v>40</v>
       </c>
-      <c r="R331" s="67" t="s">
+      <c r="R331" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S331" s="3" t="s">
@@ -35165,7 +35162,7 @@
       <c r="Q332" s="66">
         <v>40</v>
       </c>
-      <c r="R332" s="67" t="s">
+      <c r="R332" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S332" s="3" t="s">
@@ -35253,7 +35250,7 @@
       <c r="Q333" s="66">
         <v>40</v>
       </c>
-      <c r="R333" s="67" t="s">
+      <c r="R333" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S333" s="3" t="s">
@@ -35343,7 +35340,7 @@
       <c r="Q334" s="66">
         <v>40</v>
       </c>
-      <c r="R334" s="67" t="s">
+      <c r="R334" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S334" s="3" t="s">
@@ -35423,7 +35420,7 @@
       <c r="Q335" s="66">
         <v>40</v>
       </c>
-      <c r="R335" s="67" t="s">
+      <c r="R335" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S335" s="3" t="s">
@@ -35503,7 +35500,7 @@
       <c r="Q336" s="66">
         <v>40</v>
       </c>
-      <c r="R336" s="67" t="s">
+      <c r="R336" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S336" s="3" t="s">
@@ -35595,7 +35592,7 @@
       <c r="Q337" s="66">
         <v>40</v>
       </c>
-      <c r="R337" s="67" t="s">
+      <c r="R337" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S337" s="3" t="s">
@@ -35677,7 +35674,7 @@
       <c r="Q338" s="66">
         <v>40</v>
       </c>
-      <c r="R338" s="67" t="s">
+      <c r="R338" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S338" s="3" t="s">
@@ -35763,7 +35760,7 @@
       <c r="Q339" s="66">
         <v>40</v>
       </c>
-      <c r="R339" s="67" t="s">
+      <c r="R339" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S339" s="3" t="s">
@@ -35839,7 +35836,7 @@
       <c r="Q340" s="66">
         <v>40</v>
       </c>
-      <c r="R340" s="67" t="s">
+      <c r="R340" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S340" s="3" t="s">
@@ -35905,7 +35902,7 @@
       <c r="Q341" s="66">
         <v>132</v>
       </c>
-      <c r="R341" s="67" t="s">
+      <c r="R341" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S341" s="3" t="s">
@@ -35971,7 +35968,7 @@
       <c r="Q342" s="66">
         <v>40</v>
       </c>
-      <c r="R342" s="67" t="s">
+      <c r="R342" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S342" s="3" t="s">
@@ -36057,11 +36054,11 @@
       <c r="Q343" s="66">
         <v>43</v>
       </c>
-      <c r="R343" s="67" t="s">
+      <c r="R343" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S343" s="12">
-        <v>24100</v>
+      <c r="S343" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T343" s="13" t="s">
         <v>374</v>
@@ -36147,7 +36144,7 @@
       <c r="Q344" s="66">
         <v>40</v>
       </c>
-      <c r="R344" s="67" t="s">
+      <c r="R344" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S344" s="3" t="s">
@@ -36231,7 +36228,7 @@
       <c r="Q345" s="66">
         <v>40</v>
       </c>
-      <c r="R345" s="67" t="s">
+      <c r="R345" s="3" t="s">
         <v>1734</v>
       </c>
       <c r="S345" s="3" t="s">
@@ -36303,7 +36300,7 @@
       <c r="Q346" s="66">
         <v>132</v>
       </c>
-      <c r="R346" s="67" t="s">
+      <c r="R346" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S346" s="3" t="s">
@@ -36369,7 +36366,7 @@
       <c r="Q347" s="66">
         <v>40</v>
       </c>
-      <c r="R347" s="67" t="s">
+      <c r="R347" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S347" s="3" t="s">
@@ -36451,7 +36448,7 @@
       <c r="Q348" s="66">
         <v>40</v>
       </c>
-      <c r="R348" s="67" t="s">
+      <c r="R348" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S348" s="3" t="s">
@@ -36523,7 +36520,7 @@
       <c r="Q349" s="66">
         <v>40</v>
       </c>
-      <c r="R349" s="67" t="s">
+      <c r="R349" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S349" s="3" t="s">
@@ -36587,7 +36584,7 @@
       <c r="Q350" s="66">
         <v>40</v>
       </c>
-      <c r="R350" s="67" t="s">
+      <c r="R350" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S350" s="3" t="s">
@@ -36655,7 +36652,7 @@
       <c r="Q351" s="66">
         <v>40</v>
       </c>
-      <c r="R351" s="67" t="s">
+      <c r="R351" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S351" s="3" t="s">
@@ -36751,7 +36748,7 @@
       <c r="Q352" s="66">
         <v>40</v>
       </c>
-      <c r="R352" s="67" t="s">
+      <c r="R352" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S352" s="3" t="s">
@@ -36829,7 +36826,7 @@
       <c r="Q353" s="66">
         <v>132</v>
       </c>
-      <c r="R353" s="67" t="s">
+      <c r="R353" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S353" s="3" t="s">
@@ -36899,7 +36896,7 @@
       <c r="Q354" s="66">
         <v>40</v>
       </c>
-      <c r="R354" s="67" t="s">
+      <c r="R354" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S354" s="3" t="s">
@@ -36987,7 +36984,7 @@
       <c r="Q355" s="66">
         <v>40</v>
       </c>
-      <c r="R355" s="67" t="s">
+      <c r="R355" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S355" s="3" t="s">
@@ -37073,7 +37070,7 @@
       <c r="Q356" s="66">
         <v>40</v>
       </c>
-      <c r="R356" s="67" t="s">
+      <c r="R356" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S356" s="3" t="s">
@@ -37153,7 +37150,7 @@
       <c r="Q357" s="66">
         <v>40</v>
       </c>
-      <c r="R357" s="67" t="s">
+      <c r="R357" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S357" s="3" t="s">
@@ -37217,7 +37214,7 @@
       <c r="Q358" s="66">
         <v>40</v>
       </c>
-      <c r="R358" s="67" t="s">
+      <c r="R358" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S358" s="3" t="s">
@@ -37285,7 +37282,7 @@
       <c r="Q359" s="66">
         <v>40</v>
       </c>
-      <c r="R359" s="67" t="s">
+      <c r="R359" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S359" s="3" t="s">
@@ -37357,7 +37354,7 @@
       <c r="Q360" s="66">
         <v>40</v>
       </c>
-      <c r="R360" s="67" t="s">
+      <c r="R360" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S360" s="3" t="s">
@@ -37441,11 +37438,11 @@
       <c r="Q361" s="66">
         <v>43</v>
       </c>
-      <c r="R361" s="67" t="s">
+      <c r="R361" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S361" s="12">
-        <v>24100</v>
+      <c r="S361" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T361" s="13" t="s">
         <v>374</v>
@@ -37533,11 +37530,11 @@
       <c r="Q362" s="66">
         <v>40</v>
       </c>
-      <c r="R362" s="67" t="s">
+      <c r="R362" s="3" t="s">
         <v>1304</v>
       </c>
-      <c r="S362" s="12">
-        <v>4106</v>
+      <c r="S362" s="14" t="s">
+        <v>1305</v>
       </c>
       <c r="T362" s="13" t="s">
         <v>2153</v>
@@ -37625,7 +37622,7 @@
       <c r="Q363" s="66">
         <v>40</v>
       </c>
-      <c r="R363" s="67" t="s">
+      <c r="R363" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S363" s="3" t="s">
@@ -37695,7 +37692,7 @@
       <c r="Q364" s="66">
         <v>132</v>
       </c>
-      <c r="R364" s="67" t="s">
+      <c r="R364" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S364" s="3" t="s">
@@ -37783,7 +37780,7 @@
       <c r="Q365" s="66">
         <v>40</v>
       </c>
-      <c r="R365" s="67" t="s">
+      <c r="R365" s="3" t="s">
         <v>1905</v>
       </c>
       <c r="S365" s="3" t="s">
@@ -37867,7 +37864,7 @@
       <c r="Q366" s="66">
         <v>40</v>
       </c>
-      <c r="R366" s="67" t="s">
+      <c r="R366" s="3" t="s">
         <v>421</v>
       </c>
       <c r="S366" s="3" t="s">
@@ -37935,7 +37932,7 @@
       <c r="Q367" s="66">
         <v>40</v>
       </c>
-      <c r="R367" s="67" t="s">
+      <c r="R367" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S367" s="3" t="s">
@@ -37991,7 +37988,7 @@
       <c r="Q368" s="66">
         <v>40</v>
       </c>
-      <c r="R368" s="67" t="s">
+      <c r="R368" s="3" t="s">
         <v>1241</v>
       </c>
       <c r="S368" s="14" t="s">
@@ -38059,11 +38056,11 @@
       <c r="Q369" s="66">
         <v>43</v>
       </c>
-      <c r="R369" s="67" t="s">
+      <c r="R369" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S369" s="12">
-        <v>24100</v>
+      <c r="S369" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T369" s="13" t="s">
         <v>374</v>
@@ -38141,11 +38138,11 @@
       <c r="Q370" s="66">
         <v>43</v>
       </c>
-      <c r="R370" s="67" t="s">
+      <c r="R370" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S370" s="12">
-        <v>24100</v>
+      <c r="S370" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T370" s="13" t="s">
         <v>374</v>
@@ -38225,11 +38222,11 @@
       <c r="Q371" s="66">
         <v>43</v>
       </c>
-      <c r="R371" s="67" t="s">
+      <c r="R371" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S371" s="12">
-        <v>24100</v>
+      <c r="S371" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T371" s="13" t="s">
         <v>374</v>
@@ -38307,7 +38304,7 @@
       <c r="Q372" s="66">
         <v>40</v>
       </c>
-      <c r="R372" s="67" t="s">
+      <c r="R372" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S372" s="3" t="s">
@@ -38385,7 +38382,7 @@
       <c r="Q373" s="66">
         <v>40</v>
       </c>
-      <c r="R373" s="67" t="s">
+      <c r="R373" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S373" s="3" t="s">
@@ -38469,7 +38466,7 @@
       <c r="Q374" s="66">
         <v>40</v>
       </c>
-      <c r="R374" s="67" t="s">
+      <c r="R374" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S374" s="14" t="s">
@@ -38553,7 +38550,7 @@
       <c r="Q375" s="66">
         <v>132</v>
       </c>
-      <c r="R375" s="67" t="s">
+      <c r="R375" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S375" s="3" t="s">
@@ -38615,7 +38612,7 @@
       <c r="Q376" s="66">
         <v>40</v>
       </c>
-      <c r="R376" s="67" t="s">
+      <c r="R376" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S376" s="3" t="s">
@@ -38685,7 +38682,7 @@
       <c r="Q377" s="66">
         <v>40</v>
       </c>
-      <c r="R377" s="67" t="s">
+      <c r="R377" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S377" s="3" t="s">
@@ -38775,7 +38772,7 @@
       <c r="Q378" s="66">
         <v>40</v>
       </c>
-      <c r="R378" s="67" t="s">
+      <c r="R378" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S378" s="3" t="s">
@@ -38863,7 +38860,7 @@
       <c r="Q379" s="66">
         <v>40</v>
       </c>
-      <c r="R379" s="67" t="s">
+      <c r="R379" s="3" t="s">
         <v>2230</v>
       </c>
       <c r="S379" s="3" t="s">
@@ -38939,7 +38936,7 @@
       <c r="Q380" s="66">
         <v>132</v>
       </c>
-      <c r="R380" s="67" t="s">
+      <c r="R380" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S380" s="3" t="s">
@@ -39015,7 +39012,7 @@
       <c r="Q381" s="66">
         <v>132</v>
       </c>
-      <c r="R381" s="67" t="s">
+      <c r="R381" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S381" s="3" t="s">
@@ -39099,7 +39096,7 @@
       <c r="Q382" s="66">
         <v>40</v>
       </c>
-      <c r="R382" s="67" t="s">
+      <c r="R382" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S382" s="3" t="s">
@@ -39189,7 +39186,7 @@
       <c r="Q383" s="66">
         <v>40</v>
       </c>
-      <c r="R383" s="67" t="s">
+      <c r="R383" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S383" s="3" t="s">
@@ -39251,7 +39248,7 @@
       <c r="Q384" s="66">
         <v>40</v>
       </c>
-      <c r="R384" s="67" t="s">
+      <c r="R384" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S384" s="3" t="s">
@@ -39309,7 +39306,7 @@
       <c r="Q385" s="66">
         <v>40</v>
       </c>
-      <c r="R385" s="67" t="s">
+      <c r="R385" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S385" s="3" t="s">
@@ -39375,7 +39372,7 @@
       <c r="Q386" s="66">
         <v>40</v>
       </c>
-      <c r="R386" s="67" t="s">
+      <c r="R386" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S386" s="14" t="s">
@@ -39461,7 +39458,7 @@
       <c r="Q387" s="66">
         <v>40</v>
       </c>
-      <c r="R387" s="67" t="s">
+      <c r="R387" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S387" s="3" t="s">
@@ -39545,7 +39542,7 @@
       <c r="Q388" s="66">
         <v>40</v>
       </c>
-      <c r="R388" s="67" t="s">
+      <c r="R388" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S388" s="3" t="s">
@@ -39627,7 +39624,7 @@
       <c r="Q389" s="66">
         <v>40</v>
       </c>
-      <c r="R389" s="67" t="s">
+      <c r="R389" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S389" s="3" t="s">
@@ -39691,11 +39688,11 @@
       <c r="Q390" s="66">
         <v>43</v>
       </c>
-      <c r="R390" s="67" t="s">
+      <c r="R390" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S390" s="12">
-        <v>24100</v>
+      <c r="S390" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T390" s="13" t="s">
         <v>374</v>
@@ -39765,11 +39762,11 @@
       <c r="Q391" s="66">
         <v>40</v>
       </c>
-      <c r="R391" s="67" t="s">
+      <c r="R391" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="S391" s="12">
-        <v>4100</v>
+      <c r="S391" s="14" t="s">
+        <v>120</v>
       </c>
       <c r="T391" s="62" t="s">
         <v>121</v>
@@ -39847,7 +39844,7 @@
       <c r="Q392" s="66">
         <v>40</v>
       </c>
-      <c r="R392" s="67" t="s">
+      <c r="R392" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S392" s="3" t="s">
@@ -39913,7 +39910,7 @@
       <c r="Q393" s="66">
         <v>40</v>
       </c>
-      <c r="R393" s="67" t="s">
+      <c r="R393" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S393" s="3" t="s">
@@ -39989,7 +39986,7 @@
       <c r="Q394" s="66">
         <v>132</v>
       </c>
-      <c r="R394" s="67" t="s">
+      <c r="R394" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S394" s="3" t="s">
@@ -40073,7 +40070,7 @@
       <c r="Q395" s="66">
         <v>40</v>
       </c>
-      <c r="R395" s="67" t="s">
+      <c r="R395" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S395" s="3" t="s">
@@ -40159,7 +40156,7 @@
       <c r="Q396" s="66">
         <v>40</v>
       </c>
-      <c r="R396" s="67" t="s">
+      <c r="R396" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S396" s="3" t="s">
@@ -40245,7 +40242,7 @@
       <c r="Q397" s="66">
         <v>40</v>
       </c>
-      <c r="R397" s="67" t="s">
+      <c r="R397" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S397" s="3" t="s">
@@ -40327,7 +40324,7 @@
       <c r="Q398" s="66">
         <v>40</v>
       </c>
-      <c r="R398" s="67" t="s">
+      <c r="R398" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S398" s="3" t="s">
@@ -40397,7 +40394,7 @@
       <c r="Q399" s="66">
         <v>40</v>
       </c>
-      <c r="R399" s="67" t="s">
+      <c r="R399" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S399" s="3" t="s">
@@ -40491,7 +40488,7 @@
       <c r="Q400" s="66">
         <v>40</v>
       </c>
-      <c r="R400" s="67" t="s">
+      <c r="R400" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S400" s="3" t="s">
@@ -40575,7 +40572,7 @@
       <c r="Q401" s="66">
         <v>40</v>
       </c>
-      <c r="R401" s="67" t="s">
+      <c r="R401" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S401" s="3" t="s">
@@ -40639,11 +40636,11 @@
       <c r="Q402" s="66">
         <v>43</v>
       </c>
-      <c r="R402" s="67" t="s">
+      <c r="R402" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S402" s="12">
-        <v>24100</v>
+      <c r="S402" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T402" s="13" t="s">
         <v>374</v>
@@ -40731,7 +40728,7 @@
       <c r="Q403" s="66">
         <v>40</v>
       </c>
-      <c r="R403" s="67" t="s">
+      <c r="R403" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S403" s="3" t="s">
@@ -40813,11 +40810,11 @@
       <c r="Q404" s="66">
         <v>43</v>
       </c>
-      <c r="R404" s="67" t="s">
+      <c r="R404" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S404" s="12">
-        <v>24100</v>
+      <c r="S404" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T404" s="13" t="s">
         <v>374</v>
@@ -40901,7 +40898,7 @@
       <c r="Q405" s="66">
         <v>40</v>
       </c>
-      <c r="R405" s="67" t="s">
+      <c r="R405" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S405" s="3" t="s">
@@ -40985,7 +40982,7 @@
       <c r="Q406" s="66">
         <v>132</v>
       </c>
-      <c r="R406" s="67" t="s">
+      <c r="R406" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S406" s="3" t="s">
@@ -41067,7 +41064,7 @@
       <c r="Q407" s="66">
         <v>40</v>
       </c>
-      <c r="R407" s="67" t="s">
+      <c r="R407" s="3" t="s">
         <v>421</v>
       </c>
       <c r="S407" s="3" t="s">
@@ -41143,7 +41140,7 @@
       <c r="Q408" s="66">
         <v>40</v>
       </c>
-      <c r="R408" s="67" t="s">
+      <c r="R408" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S408" s="3" t="s">
@@ -41215,7 +41212,7 @@
       <c r="Q409" s="66">
         <v>57</v>
       </c>
-      <c r="R409" s="67">
+      <c r="R409" s="14">
         <v>57</v>
       </c>
       <c r="S409" s="3"/>
@@ -41299,7 +41296,7 @@
       <c r="Q410" s="66">
         <v>40</v>
       </c>
-      <c r="R410" s="67" t="s">
+      <c r="R410" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S410" s="3" t="s">
@@ -41381,7 +41378,7 @@
       <c r="Q411" s="66">
         <v>40</v>
       </c>
-      <c r="R411" s="67" t="s">
+      <c r="R411" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S411" s="3" t="s">
@@ -41463,7 +41460,7 @@
       <c r="Q412" s="66">
         <v>40</v>
       </c>
-      <c r="R412" s="67" t="s">
+      <c r="R412" s="3" t="s">
         <v>454</v>
       </c>
       <c r="S412" s="14" t="s">
@@ -41551,7 +41548,7 @@
       <c r="Q413" s="66">
         <v>40</v>
       </c>
-      <c r="R413" s="67" t="s">
+      <c r="R413" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S413" s="3" t="s">
@@ -41643,7 +41640,7 @@
       <c r="Q414" s="66">
         <v>40</v>
       </c>
-      <c r="R414" s="67" t="s">
+      <c r="R414" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S414" s="3" t="s">
@@ -41727,7 +41724,7 @@
       <c r="Q415" s="66">
         <v>40</v>
       </c>
-      <c r="R415" s="67" t="s">
+      <c r="R415" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S415" s="3" t="s">
@@ -41813,7 +41810,7 @@
       <c r="Q416" s="66">
         <v>40</v>
       </c>
-      <c r="R416" s="67" t="s">
+      <c r="R416" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S416" s="14" t="s">
@@ -41881,7 +41878,7 @@
       <c r="Q417" s="66">
         <v>132</v>
       </c>
-      <c r="R417" s="67" t="s">
+      <c r="R417" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S417" s="3" t="s">
@@ -41961,7 +41958,7 @@
       <c r="Q418" s="66">
         <v>40</v>
       </c>
-      <c r="R418" s="67" t="s">
+      <c r="R418" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S418" s="3" t="s">
@@ -42023,7 +42020,7 @@
       <c r="Q419" s="66">
         <v>40</v>
       </c>
-      <c r="R419" s="67" t="s">
+      <c r="R419" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S419" s="14" t="s">
@@ -42089,7 +42086,7 @@
       <c r="Q420" s="66">
         <v>40</v>
       </c>
-      <c r="R420" s="67" t="s">
+      <c r="R420" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S420" s="3" t="s">
@@ -42169,7 +42166,7 @@
       <c r="Q421" s="66">
         <v>40</v>
       </c>
-      <c r="R421" s="67" t="s">
+      <c r="R421" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S421" s="3" t="s">
@@ -42231,7 +42228,7 @@
       <c r="Q422" s="66">
         <v>40</v>
       </c>
-      <c r="R422" s="67" t="s">
+      <c r="R422" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S422" s="3" t="s">
@@ -42295,7 +42292,7 @@
       <c r="Q423" s="66">
         <v>40</v>
       </c>
-      <c r="R423" s="67" t="s">
+      <c r="R423" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S423" s="3" t="s">
@@ -42383,7 +42380,7 @@
       <c r="Q424" s="66">
         <v>40</v>
       </c>
-      <c r="R424" s="67" t="s">
+      <c r="R424" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S424" s="3" t="s">
@@ -42459,7 +42456,7 @@
       <c r="Q425" s="66">
         <v>40</v>
       </c>
-      <c r="R425" s="67" t="s">
+      <c r="R425" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S425" s="3" t="s">
@@ -42525,7 +42522,7 @@
       <c r="Q426" s="66">
         <v>40</v>
       </c>
-      <c r="R426" s="67" t="s">
+      <c r="R426" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S426" s="3" t="s">
@@ -42593,7 +42590,7 @@
       <c r="Q427" s="66">
         <v>40</v>
       </c>
-      <c r="R427" s="67" t="s">
+      <c r="R427" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S427" s="14" t="s">
@@ -42677,7 +42674,7 @@
       <c r="Q428" s="66">
         <v>40</v>
       </c>
-      <c r="R428" s="67" t="s">
+      <c r="R428" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S428" s="3" t="s">
@@ -42757,7 +42754,7 @@
       <c r="Q429" s="66">
         <v>40</v>
       </c>
-      <c r="R429" s="67" t="s">
+      <c r="R429" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S429" s="3" t="s">
@@ -42829,7 +42826,7 @@
       <c r="Q430" s="66">
         <v>40</v>
       </c>
-      <c r="R430" s="70" t="s">
+      <c r="R430" s="67" t="s">
         <v>1936</v>
       </c>
       <c r="S430" s="65" t="s">
@@ -42911,7 +42908,7 @@
       <c r="Q431" s="66">
         <v>43</v>
       </c>
-      <c r="R431" s="67" t="s">
+      <c r="R431" s="3" t="s">
         <v>1936</v>
       </c>
       <c r="S431" s="14" t="s">
@@ -42981,7 +42978,7 @@
       <c r="Q432" s="66">
         <v>40</v>
       </c>
-      <c r="R432" s="67" t="s">
+      <c r="R432" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S432" s="14" t="s">
@@ -43047,7 +43044,7 @@
       <c r="Q433" s="66">
         <v>132</v>
       </c>
-      <c r="R433" s="67" t="s">
+      <c r="R433" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S433" s="3" t="s">
@@ -43111,7 +43108,7 @@
       <c r="Q434" s="66">
         <v>40</v>
       </c>
-      <c r="R434" s="67" t="s">
+      <c r="R434" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S434" s="14" t="s">
@@ -43193,7 +43190,7 @@
       <c r="Q435" s="66">
         <v>40</v>
       </c>
-      <c r="R435" s="67" t="s">
+      <c r="R435" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S435" s="3" t="s">
@@ -43283,11 +43280,11 @@
       <c r="Q436" s="66">
         <v>43</v>
       </c>
-      <c r="R436" s="67" t="s">
+      <c r="R436" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S436" s="12">
-        <v>24100</v>
+      <c r="S436" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T436" s="13" t="s">
         <v>374</v>
@@ -43367,7 +43364,7 @@
       <c r="Q437" s="66">
         <v>43</v>
       </c>
-      <c r="R437" s="67" t="s">
+      <c r="R437" s="3" t="s">
         <v>1936</v>
       </c>
       <c r="S437" s="14" t="s">
@@ -43457,7 +43454,7 @@
       <c r="Q438" s="66">
         <v>132</v>
       </c>
-      <c r="R438" s="67" t="s">
+      <c r="R438" s="3" t="s">
         <v>2509</v>
       </c>
       <c r="S438" s="3" t="s">
@@ -43535,7 +43532,7 @@
       <c r="Q439" s="66">
         <v>40</v>
       </c>
-      <c r="R439" s="67" t="s">
+      <c r="R439" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S439" s="3" t="s">
@@ -43617,7 +43614,7 @@
       <c r="Q440" s="66">
         <v>132</v>
       </c>
-      <c r="R440" s="67" t="s">
+      <c r="R440" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S440" s="3" t="s">
@@ -43701,7 +43698,7 @@
       <c r="Q441" s="66">
         <v>40</v>
       </c>
-      <c r="R441" s="67" t="s">
+      <c r="R441" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S441" s="3" t="s">
@@ -43783,7 +43780,7 @@
       <c r="Q442" s="66">
         <v>40</v>
       </c>
-      <c r="R442" s="67" t="s">
+      <c r="R442" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S442" s="3" t="s">
@@ -43855,7 +43852,7 @@
       <c r="Q443" s="66">
         <v>43</v>
       </c>
-      <c r="R443" s="67" t="s">
+      <c r="R443" s="3" t="s">
         <v>1936</v>
       </c>
       <c r="S443" s="14" t="s">
@@ -43935,7 +43932,7 @@
       <c r="Q444" s="66">
         <v>43</v>
       </c>
-      <c r="R444" s="67" t="s">
+      <c r="R444" s="3" t="s">
         <v>1936</v>
       </c>
       <c r="S444" s="14" t="s">
@@ -44003,7 +44000,7 @@
       <c r="Q445" s="66">
         <v>43</v>
       </c>
-      <c r="R445" s="67" t="s">
+      <c r="R445" s="3" t="s">
         <v>1936</v>
       </c>
       <c r="S445" s="14" t="s">
@@ -44093,7 +44090,7 @@
       <c r="Q446" s="66">
         <v>40</v>
       </c>
-      <c r="R446" s="67" t="s">
+      <c r="R446" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S446" s="3" t="s">
@@ -44165,7 +44162,7 @@
       <c r="Q447" s="66">
         <v>40</v>
       </c>
-      <c r="R447" s="67" t="s">
+      <c r="R447" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S447" s="3" t="s">
@@ -44257,7 +44254,7 @@
       <c r="Q448" s="66">
         <v>40</v>
       </c>
-      <c r="R448" s="67" t="s">
+      <c r="R448" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S448" s="3" t="s">
@@ -44341,7 +44338,7 @@
       <c r="Q449" s="66">
         <v>40</v>
       </c>
-      <c r="R449" s="67" t="s">
+      <c r="R449" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S449" s="3" t="s">
@@ -44423,7 +44420,7 @@
       <c r="Q450" s="66">
         <v>40</v>
       </c>
-      <c r="R450" s="67" t="s">
+      <c r="R450" s="3" t="s">
         <v>2580</v>
       </c>
       <c r="S450" s="3">
@@ -44503,7 +44500,7 @@
       <c r="Q451" s="66">
         <v>40</v>
       </c>
-      <c r="R451" s="67" t="s">
+      <c r="R451" s="3" t="s">
         <v>131</v>
       </c>
       <c r="S451" s="3" t="s">
@@ -44583,7 +44580,7 @@
       <c r="Q452" s="66">
         <v>40</v>
       </c>
-      <c r="R452" s="67" t="s">
+      <c r="R452" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S452" s="3" t="s">
@@ -44643,7 +44640,7 @@
       <c r="Q453" s="66">
         <v>40</v>
       </c>
-      <c r="R453" s="67" t="s">
+      <c r="R453" s="3" t="s">
         <v>421</v>
       </c>
       <c r="S453" s="3" t="s">
@@ -44727,7 +44724,7 @@
       <c r="Q454" s="66">
         <v>40</v>
       </c>
-      <c r="R454" s="67" t="s">
+      <c r="R454" s="3" t="s">
         <v>119</v>
       </c>
       <c r="S454" s="3" t="s">
@@ -44807,7 +44804,7 @@
       <c r="Q455" s="66">
         <v>40</v>
       </c>
-      <c r="R455" s="67" t="s">
+      <c r="R455" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S455" s="3" t="s">
@@ -44875,7 +44872,7 @@
       <c r="Q456" s="66">
         <v>40</v>
       </c>
-      <c r="R456" s="67" t="s">
+      <c r="R456" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S456" s="3" t="s">
@@ -44965,7 +44962,7 @@
       <c r="Q457" s="66">
         <v>40</v>
       </c>
-      <c r="R457" s="67" t="s">
+      <c r="R457" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S457" s="3" t="s">
@@ -45035,11 +45032,11 @@
       <c r="Q458" s="66">
         <v>43</v>
       </c>
-      <c r="R458" s="67" t="s">
+      <c r="R458" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="S458" s="12">
-        <v>24100</v>
+      <c r="S458" s="14" t="s">
+        <v>381</v>
       </c>
       <c r="T458" s="13" t="s">
         <v>374</v>
@@ -45091,7 +45088,7 @@
       <c r="Q459" s="66">
         <v>40</v>
       </c>
-      <c r="R459" s="67" t="s">
+      <c r="R459" s="3" t="s">
         <v>2620</v>
       </c>
       <c r="S459" s="3" t="s">
@@ -45155,7 +45152,7 @@
       <c r="Q460" s="66">
         <v>40</v>
       </c>
-      <c r="R460" s="67" t="s">
+      <c r="R460" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S460" s="3" t="s">
@@ -45217,7 +45214,7 @@
       <c r="Q461" s="66">
         <v>40</v>
       </c>
-      <c r="R461" s="67" t="s">
+      <c r="R461" s="3" t="s">
         <v>2636</v>
       </c>
       <c r="S461" s="3" t="s">

</xml_diff>